<commit_message>
did an analysis of the effect of VO2 value has on the resulting metabolic power for welk001. turns out it makes a little over 1 W/kg difference. MSE comes down from 1.47 to 1.12 W/kg for the overall.
</commit_message>
<xml_diff>
--- a/metaboliccostcomparisons.xlsx
+++ b/metaboliccostcomparisons.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="64">
   <si>
     <t xml:space="preserve">t-Test: Paired Two Sample for Means</t>
   </si>
@@ -185,6 +185,9 @@
     <t xml:space="preserve">welk004</t>
   </si>
   <si>
+    <t xml:space="preserve">testing metabolics vo2 diff 1.12 w/kg</t>
+  </si>
+  <si>
     <t xml:space="preserve">experiment minus standing (average)</t>
   </si>
   <si>
@@ -207,6 +210,12 @@
   </si>
   <si>
     <t xml:space="preserve">metabolics_swing_avg_mean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE</t>
   </si>
 </sst>
 </file>
@@ -386,7 +395,7 @@
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF7E0021"/>
       <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
@@ -439,7 +448,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -851,11 +860,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="78931851"/>
-        <c:axId val="7230811"/>
+        <c:axId val="35039902"/>
+        <c:axId val="84863063"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="78931851"/>
+        <c:axId val="35039902"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="8"/>
@@ -932,12 +941,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7230811"/>
+        <c:crossAx val="84863063"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="7230811"/>
+        <c:axId val="84863063"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="14"/>
@@ -1015,7 +1024,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="78931851"/>
+        <c:crossAx val="35039902"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1067,7 +1076,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1479,11 +1488,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="84722433"/>
-        <c:axId val="46941267"/>
+        <c:axId val="79183298"/>
+        <c:axId val="93301900"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="84722433"/>
+        <c:axId val="79183298"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="13"/>
@@ -1561,12 +1570,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46941267"/>
+        <c:crossAx val="93301900"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="46941267"/>
+        <c:axId val="93301900"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="13"/>
@@ -1644,7 +1653,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84722433"/>
+        <c:crossAx val="79183298"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
@@ -1697,7 +1706,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1892,11 +1901,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="70889170"/>
-        <c:axId val="49638250"/>
+        <c:axId val="15450179"/>
+        <c:axId val="57823873"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="70889170"/>
+        <c:axId val="15450179"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1932,8 +1941,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.511328270882609"/>
-              <c:y val="0.831272514847629"/>
+              <c:x val="0.511285207983585"/>
+              <c:y val="0.831158714703019"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1970,7 +1979,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49638250"/>
+        <c:crossAx val="57823873"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1978,7 +1987,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="49638250"/>
+        <c:axId val="57823873"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2051,7 +2060,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="70889170"/>
+        <c:crossAx val="15450179"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2103,7 +2112,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart40.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2264,11 +2273,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="59515104"/>
-        <c:axId val="34955532"/>
+        <c:axId val="238834"/>
+        <c:axId val="2167892"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="59515104"/>
+        <c:axId val="238834"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2300,7 +2309,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="34955532"/>
+        <c:crossAx val="2167892"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2308,7 +2317,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="34955532"/>
+        <c:axId val="2167892"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2347,7 +2356,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="59515104"/>
+        <c:crossAx val="238834"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2375,7 +2384,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2787,11 +2796,99 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="43423631"/>
-        <c:axId val="94776201"/>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>"Subject 01 Altered"</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Subject 01 Altered</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="7e0021"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>alldata_1step!$J$2:$J$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>9.5513375</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.3817645</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>alldata_1step!$H$2:$H$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>9.941008</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.156055</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="64442680"/>
+        <c:axId val="13300090"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="43423631"/>
+        <c:axId val="64442680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="8"/>
@@ -2868,12 +2965,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94776201"/>
+        <c:crossAx val="13300090"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="94776201"/>
+        <c:axId val="13300090"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="14"/>
@@ -2951,7 +3048,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43423631"/>
+        <c:crossAx val="64442680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3003,7 +3100,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3144,6 +3241,94 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
+              <c:f>"Subject 01 Altered"</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Subject 01 Altered</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="7e0021"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7e0021"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr wrap="none"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:separator> </c:separator>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>alldata_1step!$K$2:$K$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>8.3513375</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.1817645</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>alldata_1step!$H$2:$H$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>9.941008</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.156055</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
               <c:f>"Subject 02"</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
@@ -3232,8 +3417,8 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:idx val="3"/>
+          <c:order val="3"/>
           <c:tx>
             <c:strRef>
               <c:f>"Subject 03"</c:f>
@@ -3324,8 +3509,8 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
+          <c:idx val="4"/>
+          <c:order val="4"/>
           <c:tx>
             <c:strRef>
               <c:f>"Subject 04"</c:f>
@@ -3415,11 +3600,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="37138423"/>
-        <c:axId val="87857890"/>
+        <c:axId val="91396902"/>
+        <c:axId val="40228781"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="37138423"/>
+        <c:axId val="91396902"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="13"/>
@@ -3497,12 +3682,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="87857890"/>
+        <c:crossAx val="40228781"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="87857890"/>
+        <c:axId val="40228781"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="13"/>
@@ -3580,7 +3765,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="37138423"/>
+        <c:crossAx val="91396902"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="1"/>
@@ -3633,7 +3818,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3828,11 +4013,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="48537844"/>
-        <c:axId val="57055653"/>
+        <c:axId val="97101283"/>
+        <c:axId val="40845396"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="48537844"/>
+        <c:axId val="97101283"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3868,8 +4053,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.511360099595394"/>
-              <c:y val="0.83130263393657"/>
+              <c:x val="0.511317000373088"/>
+              <c:y val="0.831197921333214"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -3906,7 +4091,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57055653"/>
+        <c:crossAx val="40845396"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3914,7 +4099,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="57055653"/>
+        <c:axId val="40845396"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3987,7 +4172,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="48537844"/>
+        <c:crossAx val="97101283"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4039,7 +4224,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4200,11 +4385,11 @@
         </c:ser>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="38678725"/>
-        <c:axId val="53106242"/>
+        <c:axId val="54894627"/>
+        <c:axId val="65682331"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="38678725"/>
+        <c:axId val="54894627"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4236,7 +4421,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53106242"/>
+        <c:crossAx val="65682331"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4244,7 +4429,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53106242"/>
+        <c:axId val="65682331"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4283,7 +4468,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38678725"/>
+        <c:crossAx val="54894627"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4322,9 +4507,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>1350360</xdr:colOff>
+      <xdr:colOff>1350000</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>56160</xdr:rowOff>
+      <xdr:rowOff>55800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4332,8 +4517,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9274320" y="3876120"/>
-        <a:ext cx="8534520" cy="5895360"/>
+        <a:off x="9273240" y="3876120"/>
+        <a:ext cx="8533800" cy="5895000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4352,9 +4537,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>310320</xdr:colOff>
+      <xdr:colOff>309960</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>66240</xdr:rowOff>
+      <xdr:rowOff>65880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4362,8 +4547,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="17676720" y="4677120"/>
-        <a:ext cx="11044440" cy="5485320"/>
+        <a:off x="17675280" y="4677120"/>
+        <a:ext cx="11048040" cy="5484960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4382,9 +4567,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
-      <xdr:colOff>90720</xdr:colOff>
+      <xdr:colOff>90360</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>12960</xdr:rowOff>
+      <xdr:rowOff>12600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4392,8 +4577,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="28865160" y="5459760"/>
-        <a:ext cx="5783400" cy="3697200"/>
+        <a:off x="28867680" y="5459760"/>
+        <a:ext cx="5789520" cy="3696840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4412,9 +4597,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>367200</xdr:colOff>
+      <xdr:colOff>366840</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>163440</xdr:rowOff>
+      <xdr:rowOff>163080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4423,7 +4608,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="25993800" y="87840"/>
-        <a:ext cx="4628520" cy="2742480"/>
+        <a:ext cx="4632480" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4441,15 +4626,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>506520</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>20880</xdr:rowOff>
+      <xdr:colOff>500040</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>44280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>700200</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>118080</xdr:colOff>
       <xdr:row>56</xdr:row>
-      <xdr:rowOff>140040</xdr:rowOff>
+      <xdr:rowOff>147240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4457,8 +4642,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11532960" y="3876480"/>
-        <a:ext cx="8609400" cy="6413400"/>
+        <a:off x="11710800" y="3724560"/>
+        <a:ext cx="5938200" cy="6572520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4479,7 +4664,7 @@
       <xdr:col>23</xdr:col>
       <xdr:colOff>505440</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>43560</xdr:rowOff>
+      <xdr:rowOff>43200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4487,8 +4672,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="20855160" y="4044960"/>
-        <a:ext cx="11518920" cy="5957640"/>
+        <a:off x="21040200" y="4044960"/>
+        <a:ext cx="11522520" cy="5957280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4503,11 +4688,11 @@
       <xdr:col>23</xdr:col>
       <xdr:colOff>455040</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>27720</xdr:rowOff>
+      <xdr:rowOff>28080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
-      <xdr:colOff>91440</xdr:colOff>
+      <xdr:colOff>91080</xdr:colOff>
       <xdr:row>52</xdr:row>
       <xdr:rowOff>90720</xdr:rowOff>
     </xdr:to>
@@ -4517,8 +4702,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="32323680" y="5460480"/>
-        <a:ext cx="5783040" cy="4017960"/>
+        <a:off x="32512320" y="5460840"/>
+        <a:ext cx="5789160" cy="4017600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4537,9 +4722,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>367920</xdr:colOff>
+      <xdr:colOff>367560</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>94680</xdr:rowOff>
+      <xdr:rowOff>94320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4547,8 +4732,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="29451960" y="87840"/>
-        <a:ext cx="4628520" cy="2986200"/>
+        <a:off x="29638080" y="87840"/>
+        <a:ext cx="4632480" cy="2985840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4572,10 +4757,10 @@
       <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.52"/>
   </cols>
@@ -4849,12 +5034,12 @@
       <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.72"/>
   </cols>
@@ -5125,18 +5310,18 @@
       <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="31.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="21.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="24.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="24.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="29.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="28.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="29.86"/>
@@ -6380,20 +6565,21 @@
   </sheetPr>
   <dimension ref="B1:BE34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N19" activeCellId="0" sqref="N19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K13" activeCellId="0" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="31.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="34.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="21.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="27.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="29.71"/>
@@ -6422,14 +6608,17 @@
       <c r="G1" s="0" t="s">
         <v>26</v>
       </c>
+      <c r="H1" s="0" t="s">
+        <v>53</v>
+      </c>
       <c r="I1" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="L1" s="0" t="s">
         <v>30</v>
@@ -6438,7 +6627,7 @@
         <v>31</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="O1" s="0" t="s">
         <v>33</v>
@@ -6474,10 +6663,10 @@
         <v>38</v>
       </c>
       <c r="AT1" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="BA1" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6500,6 +6689,10 @@
       <c r="G2" s="0" t="n">
         <v>11.061008</v>
       </c>
+      <c r="H2" s="0" t="n">
+        <f aca="false">G2-1.12</f>
+        <v>9.941008</v>
+      </c>
       <c r="I2" s="0" t="n">
         <f aca="false">G2</f>
         <v>11.061008</v>
@@ -6569,7 +6762,7 @@
         <v>23</v>
       </c>
       <c r="AX2" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="BB2" s="0" t="s">
         <v>21</v>
@@ -6581,7 +6774,7 @@
         <v>23</v>
       </c>
       <c r="BE2" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6600,6 +6793,10 @@
       <c r="G3" s="0" t="n">
         <v>11.061008</v>
       </c>
+      <c r="H3" s="0" t="n">
+        <f aca="false">G6-1.12</f>
+        <v>10.156055</v>
+      </c>
       <c r="I3" s="0" t="n">
         <f aca="false">G6</f>
         <v>11.276055</v>
@@ -7239,6 +7436,18 @@
       <c r="G11" s="0" t="n">
         <v>8.972911</v>
       </c>
+      <c r="I11" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="K11" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="L11" s="0" t="s">
+        <v>63</v>
+      </c>
       <c r="AH11" s="0" t="n">
         <v>3.085039</v>
       </c>
@@ -7298,6 +7507,22 @@
       <c r="G12" s="0" t="n">
         <v>8.972911</v>
       </c>
+      <c r="I12" s="0" t="n">
+        <f aca="false">AVERAGE(J12:J19)</f>
+        <v>1.46670992839971</v>
+      </c>
+      <c r="J12" s="0" t="n">
+        <f aca="false">(J2-I2)^2</f>
+        <v>2.27910501857025</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <f aca="false">AVERAGE(L12:L19)</f>
+        <v>1.10720084839971</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <f aca="false">(J2-H2)^2</f>
+        <v>0.15184309857025</v>
+      </c>
       <c r="AH12" s="0" t="n">
         <v>3.178002</v>
       </c>
@@ -7357,6 +7582,14 @@
       <c r="G13" s="0" t="n">
         <v>8.972911</v>
       </c>
+      <c r="J13" s="0" t="n">
+        <f aca="false">(J3-I3)^2</f>
+        <v>0.799755498390251</v>
+      </c>
+      <c r="L13" s="0" t="n">
+        <f aca="false">(J3-H3)^2</f>
+        <v>0.0509447783902503</v>
+      </c>
       <c r="AH13" s="0" t="n">
         <v>4.657112</v>
       </c>
@@ -7420,6 +7653,14 @@
       <c r="G14" s="0" t="n">
         <v>9.390569</v>
       </c>
+      <c r="J14" s="0" t="n">
+        <f aca="false">(J4-I4)^2</f>
+        <v>0.661133236200999</v>
+      </c>
+      <c r="L14" s="0" t="n">
+        <f aca="false">(J4-I4)^2</f>
+        <v>0.661133236200999</v>
+      </c>
       <c r="AH14" s="0" t="n">
         <v>2.859336</v>
       </c>
@@ -7479,6 +7720,14 @@
       <c r="G15" s="0" t="n">
         <v>9.390569</v>
       </c>
+      <c r="J15" s="0" t="n">
+        <f aca="false">(J5-I5)^2</f>
+        <v>1.31293039930806</v>
+      </c>
+      <c r="L15" s="0" t="n">
+        <f aca="false">(J5-I5)^2</f>
+        <v>1.31293039930806</v>
+      </c>
       <c r="AH15" s="0" t="n">
         <v>2.655495</v>
       </c>
@@ -7538,6 +7787,14 @@
       <c r="G16" s="0" t="n">
         <v>9.390569</v>
       </c>
+      <c r="J16" s="0" t="n">
+        <f aca="false">(J6-I6)^2</f>
+        <v>1.4386323249</v>
+      </c>
+      <c r="L16" s="0" t="n">
+        <f aca="false">(J6-I6)^2</f>
+        <v>1.4386323249</v>
+      </c>
       <c r="AH16" s="0" t="n">
         <v>2.870586</v>
       </c>
@@ -7597,6 +7854,14 @@
       <c r="G17" s="0" t="n">
         <v>9.390569</v>
       </c>
+      <c r="J17" s="0" t="n">
+        <f aca="false">(J7-I7)^2</f>
+        <v>1.58659027060056</v>
+      </c>
+      <c r="L17" s="0" t="n">
+        <f aca="false">(J7-I7)^2</f>
+        <v>1.58659027060056</v>
+      </c>
       <c r="AT17" s="0" t="n">
         <v>14</v>
       </c>
@@ -7649,6 +7914,14 @@
         <v>9.520653</v>
       </c>
       <c r="H18" s="5"/>
+      <c r="J18" s="0" t="n">
+        <f aca="false">(J8-I8)^2</f>
+        <v>0.129329421376</v>
+      </c>
+      <c r="L18" s="0" t="n">
+        <f aca="false">(J8-I8)^2</f>
+        <v>0.129329421376</v>
+      </c>
       <c r="AT18" s="0" t="n">
         <v>15</v>
       </c>
@@ -7697,6 +7970,14 @@
         <v>9.520653</v>
       </c>
       <c r="H19" s="5"/>
+      <c r="J19" s="0" t="n">
+        <f aca="false">(J9-I9)^2</f>
+        <v>3.52620325785157</v>
+      </c>
+      <c r="L19" s="0" t="n">
+        <f aca="false">(J9-I9)^2</f>
+        <v>3.52620325785157</v>
+      </c>
       <c r="AT19" s="0" t="n">
         <v>16</v>
       </c>
@@ -8467,7 +8748,7 @@
       <selection pane="topLeft" activeCell="P1" activeCellId="0" sqref="P1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="30.86"/>
@@ -8492,10 +8773,10 @@
         <v>26</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8527,7 +8808,7 @@
         <v>23</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="Q2" s="0" t="s">
         <v>21</v>
@@ -8539,7 +8820,7 @@
         <v>23</v>
       </c>
       <c r="T2" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
working through welk002 and welk003 solo analysis
</commit_message>
<xml_diff>
--- a/metaboliccostcomparisons.xlsx
+++ b/metaboliccostcomparisons.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\code\repos\Stanford\delplab\projects\muscleModel\muscleEnergyModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A4622E6-56D9-4117-B6FB-BF3BDA7BA0C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6242AE95-ECE1-4456-94A4-8D7C5DC13950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2570,10 +2570,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>9.5513375000000007</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.381764500000001</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2855,10 +2855,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>9.4851139999999994</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.887213750000001</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2965,10 +2965,10 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="2"/>
                       <c:pt idx="0">
-                        <c:v>9.5513375000000007</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>10.381764500000001</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3244,7 +3244,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr lang="en-US" sz="2800" b="0" strike="noStrike" spc="-1">
+              <a:defRPr lang="en-US" sz="4000" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -3252,7 +3252,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="2800" b="0" strike="noStrike" spc="-1">
+              <a:rPr lang="en-US" sz="4000" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -3342,10 +3342,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>8.3513375000000014</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.1817645000000017</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3627,10 +3627,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>8.2851140000000001</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.6872137500000015</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3654,6 +3654,62 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-91D1-475F-B172-92ACE69A5823}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>y=x</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:spPr>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:alpha val="39000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="2"/>
+              <c:pt idx="0">
+                <c:v>8</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>12</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:xVal>
+          <c:yVal>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="2"/>
+              <c:pt idx="0">
+                <c:v>8</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>12</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-1BDB-4C89-873C-2104705A413C}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3737,10 +3793,10 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="2"/>
                       <c:pt idx="0">
-                        <c:v>8.3513375000000014</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>9.1817645000000017</c:v>
+                        <c:v>0</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
@@ -3803,7 +3859,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr lang="en-US" sz="2400" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr lang="en-US" sz="3600" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -3811,7 +3867,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="2400" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="3600" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -3847,7 +3903,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="2000" b="0" strike="noStrike" spc="-1">
+              <a:defRPr sz="3200" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -3888,7 +3944,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr lang="en-US" sz="2400" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr lang="en-US" sz="3600" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -3896,7 +3952,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="2400" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="3600" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -3932,7 +3988,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="2000" b="0" strike="noStrike" spc="-1">
+              <a:defRPr sz="3200" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -3956,6 +4012,10 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:legendEntry>
+        <c:idx val="5"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3968,7 +4028,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="2000" b="0" strike="noStrike" spc="-1">
+            <a:defRPr sz="3200" b="0" strike="noStrike" spc="-1">
               <a:solidFill>
                 <a:srgbClr val="595959"/>
               </a:solidFill>
@@ -4190,7 +4250,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>-7.9989003796031017</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>-7.1218698662349267</c:v>
@@ -4199,7 +4259,7 @@
                   <c:v>-3.3261346280015869</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-12.878407480518156</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4594,7 +4654,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>-9.044307333301786</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>-8.0372380116609783</c:v>
@@ -4603,7 +4663,7 @@
                   <c:v>-3.7297543833232742</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-14.473715416881364</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7128,8 +7188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:BE34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="69" zoomScaleNormal="65" workbookViewId="0">
-      <selection activeCell="AR46" sqref="AR46"/>
+    <sheetView tabSelected="1" topLeftCell="F14" zoomScale="69" zoomScaleNormal="65" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7242,12 +7302,9 @@
       <c r="D2" t="s">
         <v>41</v>
       </c>
-      <c r="E2">
-        <v>9.3871509999999994</v>
-      </c>
-      <c r="F2">
+      <c r="F2" t="e">
         <f>AVERAGE(E2:E5)</f>
-        <v>9.5513375000000007</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="G2">
         <v>11.061007999999999</v>
@@ -7260,13 +7317,13 @@
         <f>G2</f>
         <v>11.061007999999999</v>
       </c>
-      <c r="J2">
+      <c r="J2" t="e">
         <f>F2</f>
-        <v>9.5513375000000007</v>
-      </c>
-      <c r="K2">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K2" t="e">
         <f t="shared" ref="K2:K9" si="0">J2-1.2</f>
-        <v>8.3513375000000014</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="L2">
         <v>1</v>
@@ -7275,21 +7332,21 @@
         <f>(AVERAGE(I2:I2)-AVERAGE(I3:I3))/(AVERAGE(I3:I3))*100</f>
         <v>-1.9071120174564617</v>
       </c>
-      <c r="N2">
+      <c r="N2" t="e">
         <f>(AVERAGE(J2:J2)-AVERAGE(J3:J3))/(AVERAGE(J3:J3))*100</f>
-        <v>-7.9989003796031017</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="O2">
         <f>(I2-I3)/I3*100</f>
         <v>-1.9071120174564617</v>
       </c>
-      <c r="P2">
+      <c r="P2" t="e">
         <f>(J2-J3)/J3*100</f>
-        <v>-7.9989003796031017</v>
-      </c>
-      <c r="Q2">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q2" t="e">
         <f>(K2-K3)/K3*100</f>
-        <v>-9.044307333301786</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="AG2" t="s">
         <v>42</v>
@@ -7350,9 +7407,6 @@
       <c r="D3" t="s">
         <v>44</v>
       </c>
-      <c r="E3">
-        <v>10.119400000000001</v>
-      </c>
       <c r="G3">
         <v>11.061007999999999</v>
       </c>
@@ -7364,13 +7418,13 @@
         <f>G6</f>
         <v>11.276054999999999</v>
       </c>
-      <c r="J3">
+      <c r="J3" t="e">
         <f>F6</f>
-        <v>10.381764500000001</v>
-      </c>
-      <c r="K3">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K3" t="e">
         <f t="shared" si="0"/>
-        <v>9.1817645000000017</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="L3">
         <v>2</v>
@@ -7448,9 +7502,6 @@
       <c r="D4" t="s">
         <v>45</v>
       </c>
-      <c r="E4">
-        <v>9.0773960000000002</v>
-      </c>
       <c r="G4">
         <v>11.061007999999999</v>
       </c>
@@ -7542,9 +7593,6 @@
       <c r="D5" t="s">
         <v>46</v>
       </c>
-      <c r="E5">
-        <v>9.6214030000000008</v>
-      </c>
       <c r="G5">
         <v>11.061007999999999</v>
       </c>
@@ -7567,21 +7615,21 @@
         <f>(AVERAGE(I8:I8)-AVERAGE(I9:I9))/(AVERAGE(I9:I9))*100</f>
         <v>1.2885992899634173</v>
       </c>
-      <c r="N5">
+      <c r="N5" t="e">
         <f>(AVERAGE(J8:J8)-AVERAGE(J9:J9))/(AVERAGE(J9:J9))*100</f>
-        <v>-12.878407480518156</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="O5">
         <f>(I8-I9)/I9*100</f>
         <v>1.2885992899634173</v>
       </c>
-      <c r="P5">
+      <c r="P5" t="e">
         <f>(J8-J9)/J9*100</f>
-        <v>-12.878407480518156</v>
-      </c>
-      <c r="Q5">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="Q5" t="e">
         <f>(K8-K9)/K9*100</f>
-        <v>-14.473715416881364</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="AH5">
         <v>2.670731</v>
@@ -7636,12 +7684,9 @@
       <c r="D6" t="s">
         <v>41</v>
       </c>
-      <c r="E6">
-        <v>10.156669000000001</v>
-      </c>
-      <c r="F6">
+      <c r="F6" t="e">
         <f>AVERAGE(E6:E9)</f>
-        <v>10.381764500000001</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="G6">
         <v>11.276054999999999</v>
@@ -7711,9 +7756,6 @@
       <c r="D7" t="s">
         <v>44</v>
       </c>
-      <c r="E7">
-        <v>10.552236000000001</v>
-      </c>
       <c r="G7">
         <v>11.276054999999999</v>
       </c>
@@ -7782,9 +7824,6 @@
       <c r="D8" t="s">
         <v>45</v>
       </c>
-      <c r="E8">
-        <v>10.569394000000001</v>
-      </c>
       <c r="G8">
         <v>11.276054999999999</v>
       </c>
@@ -7792,13 +7831,13 @@
         <f>G26</f>
         <v>9.1254899999999992</v>
       </c>
-      <c r="J8">
+      <c r="J8" t="e">
         <f>F26</f>
-        <v>9.4851139999999994</v>
-      </c>
-      <c r="K8">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K8" t="e">
         <f t="shared" si="0"/>
-        <v>8.2851140000000001</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="M8" t="s">
         <v>48</v>
@@ -7859,9 +7898,6 @@
       <c r="D9" t="s">
         <v>46</v>
       </c>
-      <c r="E9">
-        <v>10.248759</v>
-      </c>
       <c r="G9">
         <v>11.276054999999999</v>
       </c>
@@ -7869,13 +7905,13 @@
         <f>G30</f>
         <v>9.0093949999999996</v>
       </c>
-      <c r="J9">
+      <c r="J9" t="e">
         <f>F30</f>
-        <v>10.887213750000001</v>
-      </c>
-      <c r="K9">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K9" t="e">
         <f t="shared" si="0"/>
-        <v>9.6872137500000015</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="AH9">
         <v>3.3469850000000001</v>
@@ -8070,21 +8106,21 @@
       <c r="G12">
         <v>8.9729109999999999</v>
       </c>
-      <c r="I12">
+      <c r="I12" t="e">
         <f>AVERAGE(J12:J19)</f>
-        <v>1.4667099283997107</v>
-      </c>
-      <c r="J12">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J12" t="e">
         <f t="shared" ref="J12:J19" si="1">(J2-I2)^2</f>
-        <v>2.2791050185702457</v>
-      </c>
-      <c r="K12">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K12" t="e">
         <f>AVERAGE(L12:L19)</f>
-        <v>1.1072008483997118</v>
-      </c>
-      <c r="L12">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L12" t="e">
         <f>(J2-H2)^2</f>
-        <v>0.1518430985702495</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="AH12">
         <v>3.1780020000000002</v>
@@ -8145,13 +8181,13 @@
       <c r="G13">
         <v>8.9729109999999999</v>
       </c>
-      <c r="J13">
+      <c r="J13" t="e">
         <f t="shared" si="1"/>
-        <v>0.7997554983902474</v>
-      </c>
-      <c r="L13">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L13" t="e">
         <f>(J3-H3)^2</f>
-        <v>5.0944778390251105E-2</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="AH13">
         <v>4.6571119999999997</v>
@@ -8477,13 +8513,13 @@
         <v>9.5206529999999994</v>
       </c>
       <c r="H18" s="5"/>
-      <c r="J18">
+      <c r="J18" t="e">
         <f t="shared" si="1"/>
-        <v>0.12932942137600012</v>
-      </c>
-      <c r="L18">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L18" t="e">
         <f t="shared" si="2"/>
-        <v>0.12932942137600012</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="AT18">
         <v>15</v>
@@ -8533,13 +8569,13 @@
         <v>9.5206529999999994</v>
       </c>
       <c r="H19" s="5"/>
-      <c r="J19">
+      <c r="J19" t="e">
         <f t="shared" si="1"/>
-        <v>3.526203257851567</v>
-      </c>
-      <c r="L19">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L19" t="e">
         <f t="shared" si="2"/>
-        <v>3.526203257851567</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="AT19">
         <v>16</v>
@@ -8874,12 +8910,9 @@
       <c r="D26" t="s">
         <v>41</v>
       </c>
-      <c r="E26">
-        <v>9.584301</v>
-      </c>
-      <c r="F26">
+      <c r="F26" t="e">
         <f>AVERAGE(E26:E29)</f>
-        <v>9.4851139999999994</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="G26" s="5">
         <v>9.1254899999999992</v>
@@ -8926,9 +8959,6 @@
       <c r="D27" t="s">
         <v>44</v>
       </c>
-      <c r="E27">
-        <v>9.0162069999999996</v>
-      </c>
       <c r="G27" s="5">
         <v>9.1254899999999992</v>
       </c>
@@ -8974,9 +9004,6 @@
       <c r="D28" t="s">
         <v>45</v>
       </c>
-      <c r="E28">
-        <v>9.5586479999999998</v>
-      </c>
       <c r="G28" s="5">
         <v>9.1254899999999992</v>
       </c>
@@ -9022,9 +9049,6 @@
       <c r="D29" t="s">
         <v>46</v>
       </c>
-      <c r="E29">
-        <v>9.7812999999999999</v>
-      </c>
       <c r="G29" s="5">
         <v>9.1254899999999992</v>
       </c>
@@ -9070,12 +9094,9 @@
       <c r="D30" t="s">
         <v>41</v>
       </c>
-      <c r="E30">
-        <v>13.220052000000001</v>
-      </c>
-      <c r="F30">
+      <c r="F30" t="e">
         <f>AVERAGE(E30:E33)</f>
-        <v>10.887213750000001</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="G30" s="5">
         <v>9.0093949999999996</v>
@@ -9122,9 +9143,6 @@
       <c r="D31" t="s">
         <v>44</v>
       </c>
-      <c r="E31">
-        <v>9.8514009999999992</v>
-      </c>
       <c r="G31" s="5">
         <v>9.0093949999999996</v>
       </c>
@@ -9170,9 +9188,6 @@
       <c r="D32" t="s">
         <v>45</v>
       </c>
-      <c r="E32">
-        <v>10.149334</v>
-      </c>
       <c r="G32" s="5">
         <v>9.0093949999999996</v>
       </c>
@@ -9217,9 +9232,6 @@
       </c>
       <c r="D33" t="s">
         <v>46</v>
-      </c>
-      <c r="E33">
-        <v>10.328068</v>
       </c>
       <c r="G33" s="5">
         <v>9.0093949999999996</v>

</xml_diff>

<commit_message>
working through the 2 subject analysis.
</commit_message>
<xml_diff>
--- a/metaboliccostcomparisons.xlsx
+++ b/metaboliccostcomparisons.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\code\repos\Stanford\delplab\projects\muscleModel\muscleEnergyModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6242AE95-ECE1-4456-94A4-8D7C5DC13950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC67559-04F3-4D51-811E-961D655CA7E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4076,7 +4076,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr lang="en-US" sz="2800" b="0" strike="noStrike" spc="-1">
+              <a:defRPr lang="en-US" sz="4000" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -4084,7 +4084,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="2800" b="0" strike="noStrike" spc="-1">
+              <a:rPr lang="en-US" sz="4000" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -4163,23 +4163,40 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="2"/>
+              <c:pt idx="0">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>3</c:v>
+              </c:pt>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:autoCat val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:strLit>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>alldata_1step!$M$2:$M$5</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>alldata_1step!$M$2:$M$5</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>alldata_1step!$M$3:$M$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>-1.9071120174564617</c:v>
+                  <c:v>-4.4476325130031995</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-4.4476325130031995</c:v>
-                </c:pt>
-                <c:pt idx="2">
                   <c:v>-3.1402286791878598</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.2885992899634173</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4243,23 +4260,40 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="2"/>
+              <c:pt idx="0">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>3</c:v>
+              </c:pt>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:autoCat val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:strLit>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>alldata_1step!$N$2:$N$5</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>alldata_1step!$N$2:$N$5</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>alldata_1step!$N$3:$N$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>-7.1218698662349267</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-7.1218698662349267</c:v>
-                </c:pt>
-                <c:pt idx="2">
                   <c:v>-3.3261346280015869</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4297,7 +4331,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr lang="en-US" sz="2000" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr lang="en-US" sz="3600" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -4305,7 +4339,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="2000" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="3600" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -4349,7 +4383,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="2400" b="0" strike="noStrike" spc="-1">
+              <a:defRPr sz="3200" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -4390,7 +4424,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr lang="en-US" sz="2400" b="0" strike="noStrike" spc="-1">
+                  <a:defRPr lang="en-US" sz="3600" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -4398,7 +4432,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="2400" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="3600" b="0" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="595959"/>
                     </a:solidFill>
@@ -4431,7 +4465,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="2000" b="0" strike="noStrike" spc="-1">
+              <a:defRPr sz="3200" b="0" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="595959"/>
                 </a:solidFill>
@@ -7188,7 +7222,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:BE34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F14" zoomScale="69" zoomScaleNormal="65" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="P11" zoomScale="69" zoomScaleNormal="65" workbookViewId="0">
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
need to figure out the stance and swing stats
</commit_message>
<xml_diff>
--- a/metaboliccostcomparisons.xlsx
+++ b/metaboliccostcomparisons.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\code\repos\Stanford\delplab\projects\muscleModel\muscleEnergyModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB154D3A-D036-4EC9-AF13-69A2123B73BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655AE7FC-58FB-4EFC-8682-276515398B80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" tabRatio="500" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="alldata" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="87">
   <si>
     <t>t-Test: Paired Two Sample for Means</t>
   </si>
@@ -7430,7 +7430,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFB71C57-F672-4F0F-AF5A-E40E874EA6E6}">
   <dimension ref="A1:S32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A18" sqref="A18:A20"/>
     </sheetView>
   </sheetViews>
@@ -8028,10 +8028,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B1:BE34"/>
+  <dimension ref="B1:Q33"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="67" zoomScaleNormal="65" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="67" zoomScaleNormal="65" workbookViewId="0">
+      <selection activeCell="AG1" sqref="AG1:AQ16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8054,7 +8054,7 @@
     <col min="17" max="17" width="29.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:57" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>14</v>
       </c>
@@ -8103,38 +8103,8 @@
       <c r="Q1" t="s">
         <v>28</v>
       </c>
-      <c r="AG1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AH1">
-        <v>3.3153860000000002</v>
-      </c>
-      <c r="AJ1">
-        <v>2.9823819999999999</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AN1">
-        <v>6.1065969999999998</v>
-      </c>
-      <c r="AP1">
-        <v>5.7093870000000004</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>51</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="2:57" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>32</v>
       </c>
@@ -8190,56 +8160,8 @@
         <f>(K2-K3)/K3*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AG2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH2">
-        <v>3.2434959999999999</v>
-      </c>
-      <c r="AJ2">
-        <v>2.9537140000000002</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AN2">
-        <v>6.7520709999999999</v>
-      </c>
-      <c r="AP2">
-        <v>6.6018739999999996</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>14</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>15</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>16</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>53</v>
-      </c>
-      <c r="BB2" t="s">
-        <v>14</v>
-      </c>
-      <c r="BC2" t="s">
-        <v>15</v>
-      </c>
-      <c r="BD2" t="s">
-        <v>16</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="2:57" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>32</v>
       </c>
@@ -8291,50 +8213,8 @@
         <f>(K4-K5)/(K5)*100</f>
         <v>-8.0372380116609783</v>
       </c>
-      <c r="AH3">
-        <v>3.3281550000000002</v>
-      </c>
-      <c r="AJ3">
-        <v>2.9966629999999999</v>
-      </c>
-      <c r="AN3">
-        <v>6.5153059999999998</v>
-      </c>
-      <c r="AP3">
-        <v>5.2269589999999999</v>
-      </c>
-      <c r="AT3">
-        <v>0</v>
-      </c>
-      <c r="AU3" t="s">
-        <v>32</v>
-      </c>
-      <c r="AV3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AW3" t="s">
-        <v>34</v>
-      </c>
-      <c r="AX3">
-        <v>5.7093870000000004</v>
-      </c>
-      <c r="BA3">
-        <v>0</v>
-      </c>
-      <c r="BB3" t="s">
-        <v>32</v>
-      </c>
-      <c r="BC3" t="s">
-        <v>33</v>
-      </c>
-      <c r="BD3" t="s">
-        <v>34</v>
-      </c>
-      <c r="BE3">
-        <v>2.9823819999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="2:57" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>32</v>
       </c>
@@ -8382,50 +8262,8 @@
         <f>(K6-K7)/K7*100</f>
         <v>-3.7297543833232742</v>
       </c>
-      <c r="AH4">
-        <v>3.2258420000000001</v>
-      </c>
-      <c r="AJ4">
-        <v>2.957643</v>
-      </c>
-      <c r="AN4">
-        <v>6.4289120000000004</v>
-      </c>
-      <c r="AP4">
-        <v>6.045452</v>
-      </c>
-      <c r="AT4">
-        <v>1</v>
-      </c>
-      <c r="AU4" t="s">
-        <v>32</v>
-      </c>
-      <c r="AV4" t="s">
-        <v>33</v>
-      </c>
-      <c r="AW4" t="s">
-        <v>37</v>
-      </c>
-      <c r="AX4">
-        <v>6.6018739999999996</v>
-      </c>
-      <c r="BA4">
-        <v>1</v>
-      </c>
-      <c r="BB4" t="s">
-        <v>32</v>
-      </c>
-      <c r="BC4" t="s">
-        <v>33</v>
-      </c>
-      <c r="BD4" t="s">
-        <v>37</v>
-      </c>
-      <c r="BE4">
-        <v>2.9537140000000002</v>
-      </c>
-    </row>
-    <row r="5" spans="2:57" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>32</v>
       </c>
@@ -8473,50 +8311,8 @@
         <f>(K8-K9)/K9*100</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AH5">
-        <v>2.670731</v>
-      </c>
-      <c r="AJ5">
-        <v>2.8224860000000001</v>
-      </c>
-      <c r="AN5">
-        <v>7.4643920000000001</v>
-      </c>
-      <c r="AP5">
-        <v>6.6376109999999997</v>
-      </c>
-      <c r="AT5">
-        <v>2</v>
-      </c>
-      <c r="AU5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AV5" t="s">
-        <v>33</v>
-      </c>
-      <c r="AW5" t="s">
-        <v>38</v>
-      </c>
-      <c r="AX5">
-        <v>5.2269589999999999</v>
-      </c>
-      <c r="BA5">
-        <v>2</v>
-      </c>
-      <c r="BB5" t="s">
-        <v>32</v>
-      </c>
-      <c r="BC5" t="s">
-        <v>33</v>
-      </c>
-      <c r="BD5" t="s">
-        <v>38</v>
-      </c>
-      <c r="BE5">
-        <v>2.9966629999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="2:57" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>32</v>
       </c>
@@ -8545,50 +8341,8 @@
         <f t="shared" si="0"/>
         <v>9.5200830000000014</v>
       </c>
-      <c r="AH6">
-        <v>3.1026220000000002</v>
-      </c>
-      <c r="AJ6">
-        <v>2.7806150000000001</v>
-      </c>
-      <c r="AN6">
-        <v>7.6236660000000001</v>
-      </c>
-      <c r="AP6">
-        <v>5.9639850000000001</v>
-      </c>
-      <c r="AT6">
-        <v>3</v>
-      </c>
-      <c r="AU6" t="s">
-        <v>32</v>
-      </c>
-      <c r="AV6" t="s">
-        <v>33</v>
-      </c>
-      <c r="AW6" t="s">
-        <v>39</v>
-      </c>
-      <c r="AX6">
-        <v>6.045452</v>
-      </c>
-      <c r="BA6">
-        <v>3</v>
-      </c>
-      <c r="BB6" t="s">
-        <v>32</v>
-      </c>
-      <c r="BC6" t="s">
-        <v>33</v>
-      </c>
-      <c r="BD6" t="s">
-        <v>39</v>
-      </c>
-      <c r="BE6">
-        <v>2.957643</v>
-      </c>
-    </row>
-    <row r="7" spans="2:57" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>32</v>
       </c>
@@ -8613,50 +8367,8 @@
         <f t="shared" si="0"/>
         <v>9.8889152500000002</v>
       </c>
-      <c r="AH7">
-        <v>2.6562060000000001</v>
-      </c>
-      <c r="AJ7">
-        <v>2.5526460000000002</v>
-      </c>
-      <c r="AN7">
-        <v>6.9179539999999999</v>
-      </c>
-      <c r="AP7">
-        <v>6.6552610000000003</v>
-      </c>
-      <c r="AT7">
-        <v>4</v>
-      </c>
-      <c r="AU7" t="s">
-        <v>32</v>
-      </c>
-      <c r="AV7" t="s">
-        <v>40</v>
-      </c>
-      <c r="AW7" t="s">
-        <v>34</v>
-      </c>
-      <c r="AX7">
-        <v>6.1065969999999998</v>
-      </c>
-      <c r="BA7">
-        <v>4</v>
-      </c>
-      <c r="BB7" t="s">
-        <v>32</v>
-      </c>
-      <c r="BC7" t="s">
-        <v>40</v>
-      </c>
-      <c r="BD7" t="s">
-        <v>34</v>
-      </c>
-      <c r="BE7">
-        <v>3.3153860000000002</v>
-      </c>
-    </row>
-    <row r="8" spans="2:57" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>32</v>
       </c>
@@ -8687,50 +8399,8 @@
       <c r="O8" t="s">
         <v>42</v>
       </c>
-      <c r="AH8">
-        <v>2.774289</v>
-      </c>
-      <c r="AJ8">
-        <v>2.8426930000000001</v>
-      </c>
-      <c r="AN8">
-        <v>6.8632220000000004</v>
-      </c>
-      <c r="AP8">
-        <v>5.8253329999999997</v>
-      </c>
-      <c r="AT8">
-        <v>5</v>
-      </c>
-      <c r="AU8" t="s">
-        <v>32</v>
-      </c>
-      <c r="AV8" t="s">
-        <v>40</v>
-      </c>
-      <c r="AW8" t="s">
-        <v>37</v>
-      </c>
-      <c r="AX8">
-        <v>6.7520709999999999</v>
-      </c>
-      <c r="BA8">
-        <v>5</v>
-      </c>
-      <c r="BB8" t="s">
-        <v>32</v>
-      </c>
-      <c r="BC8" t="s">
-        <v>40</v>
-      </c>
-      <c r="BD8" t="s">
-        <v>37</v>
-      </c>
-      <c r="BE8">
-        <v>3.2434959999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="2:57" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>32</v>
       </c>
@@ -8755,50 +8425,8 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AH9">
-        <v>3.3469850000000001</v>
-      </c>
-      <c r="AJ9">
-        <v>3.190118</v>
-      </c>
-      <c r="AN9">
-        <v>7.3225720000000001</v>
-      </c>
-      <c r="AP9">
-        <v>6.9033720000000001</v>
-      </c>
-      <c r="AT9">
-        <v>6</v>
-      </c>
-      <c r="AU9" t="s">
-        <v>32</v>
-      </c>
-      <c r="AV9" t="s">
-        <v>40</v>
-      </c>
-      <c r="AW9" t="s">
-        <v>38</v>
-      </c>
-      <c r="AX9">
-        <v>6.5153059999999998</v>
-      </c>
-      <c r="BA9">
-        <v>6</v>
-      </c>
-      <c r="BB9" t="s">
-        <v>32</v>
-      </c>
-      <c r="BC9" t="s">
-        <v>40</v>
-      </c>
-      <c r="BD9" t="s">
-        <v>38</v>
-      </c>
-      <c r="BE9">
-        <v>3.3281550000000002</v>
-      </c>
-    </row>
-    <row r="10" spans="2:57" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>43</v>
       </c>
@@ -8818,50 +8446,8 @@
       <c r="G10">
         <v>8.9729109999999999</v>
       </c>
-      <c r="AH10">
-        <v>3.0652469999999998</v>
-      </c>
-      <c r="AJ10">
-        <v>3.1468889999999998</v>
-      </c>
-      <c r="AN10">
-        <v>7.7138470000000003</v>
-      </c>
-      <c r="AP10">
-        <v>6.647322</v>
-      </c>
-      <c r="AT10">
-        <v>7</v>
-      </c>
-      <c r="AU10" t="s">
-        <v>32</v>
-      </c>
-      <c r="AV10" t="s">
-        <v>40</v>
-      </c>
-      <c r="AW10" t="s">
-        <v>39</v>
-      </c>
-      <c r="AX10">
-        <v>6.4289120000000004</v>
-      </c>
-      <c r="BA10">
-        <v>7</v>
-      </c>
-      <c r="BB10" t="s">
-        <v>32</v>
-      </c>
-      <c r="BC10" t="s">
-        <v>40</v>
-      </c>
-      <c r="BD10" t="s">
-        <v>39</v>
-      </c>
-      <c r="BE10">
-        <v>3.2258420000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="2:57" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>43</v>
       </c>
@@ -8889,50 +8475,8 @@
       <c r="L11" t="s">
         <v>56</v>
       </c>
-      <c r="AH11">
-        <v>3.0850390000000001</v>
-      </c>
-      <c r="AJ11">
-        <v>3.2110289999999999</v>
-      </c>
-      <c r="AN11">
-        <v>7.5333889999999997</v>
-      </c>
-      <c r="AP11">
-        <v>6.3015169999999996</v>
-      </c>
-      <c r="AT11">
-        <v>8</v>
-      </c>
-      <c r="AU11" t="s">
-        <v>43</v>
-      </c>
-      <c r="AV11" t="s">
-        <v>33</v>
-      </c>
-      <c r="AW11" t="s">
-        <v>34</v>
-      </c>
-      <c r="AX11">
-        <v>6.6376109999999997</v>
-      </c>
-      <c r="BA11">
-        <v>8</v>
-      </c>
-      <c r="BB11" t="s">
-        <v>43</v>
-      </c>
-      <c r="BC11" t="s">
-        <v>33</v>
-      </c>
-      <c r="BD11" t="s">
-        <v>34</v>
-      </c>
-      <c r="BE11">
-        <v>2.8224860000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="2:57" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>43</v>
       </c>
@@ -8964,50 +8508,8 @@
         <f>(J2-H2)^2</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AH12">
-        <v>3.1780020000000002</v>
-      </c>
-      <c r="AJ12">
-        <v>3.5255000000000001</v>
-      </c>
-      <c r="AN12">
-        <v>7.8034150000000002</v>
-      </c>
-      <c r="AP12">
-        <v>6.898752</v>
-      </c>
-      <c r="AT12">
-        <v>9</v>
-      </c>
-      <c r="AU12" t="s">
-        <v>43</v>
-      </c>
-      <c r="AV12" t="s">
-        <v>33</v>
-      </c>
-      <c r="AW12" t="s">
-        <v>37</v>
-      </c>
-      <c r="AX12">
-        <v>5.9639850000000001</v>
-      </c>
-      <c r="BA12">
-        <v>9</v>
-      </c>
-      <c r="BB12" t="s">
-        <v>43</v>
-      </c>
-      <c r="BC12" t="s">
-        <v>33</v>
-      </c>
-      <c r="BD12" t="s">
-        <v>37</v>
-      </c>
-      <c r="BE12">
-        <v>2.7806150000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="2:57" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>43</v>
       </c>
@@ -9031,50 +8533,8 @@
         <f>(J3-H3)^2</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AH13">
-        <v>4.6571119999999997</v>
-      </c>
-      <c r="AJ13">
-        <v>2.9394070000000001</v>
-      </c>
-      <c r="AN13">
-        <v>8.0594289999999997</v>
-      </c>
-      <c r="AP13">
-        <v>6.1153700000000004</v>
-      </c>
-      <c r="AT13">
-        <v>10</v>
-      </c>
-      <c r="AU13" t="s">
-        <v>43</v>
-      </c>
-      <c r="AV13" t="s">
-        <v>33</v>
-      </c>
-      <c r="AW13" t="s">
-        <v>38</v>
-      </c>
-      <c r="AX13">
-        <v>6.6552610000000003</v>
-      </c>
-      <c r="BA13">
-        <v>10</v>
-      </c>
-      <c r="BB13" t="s">
-        <v>43</v>
-      </c>
-      <c r="BC13" t="s">
-        <v>33</v>
-      </c>
-      <c r="BD13" t="s">
-        <v>38</v>
-      </c>
-      <c r="BE13">
-        <v>2.5526460000000002</v>
-      </c>
-    </row>
-    <row r="14" spans="2:57" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>43</v>
       </c>
@@ -9102,50 +8562,8 @@
         <f t="shared" ref="L14:L19" si="2">(J4-I4)^2</f>
         <v>0.6611332362009994</v>
       </c>
-      <c r="AH14">
-        <v>2.8593359999999999</v>
-      </c>
-      <c r="AJ14">
-        <v>2.7081900000000001</v>
-      </c>
-      <c r="AN14">
-        <v>6.5402509999999996</v>
-      </c>
-      <c r="AP14">
-        <v>5.5948729999999998</v>
-      </c>
-      <c r="AT14">
-        <v>11</v>
-      </c>
-      <c r="AU14" t="s">
-        <v>43</v>
-      </c>
-      <c r="AV14" t="s">
-        <v>33</v>
-      </c>
-      <c r="AW14" t="s">
-        <v>39</v>
-      </c>
-      <c r="AX14">
-        <v>5.8253329999999997</v>
-      </c>
-      <c r="BA14">
-        <v>11</v>
-      </c>
-      <c r="BB14" t="s">
-        <v>43</v>
-      </c>
-      <c r="BC14" t="s">
-        <v>33</v>
-      </c>
-      <c r="BD14" t="s">
-        <v>39</v>
-      </c>
-      <c r="BE14">
-        <v>2.8426930000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="2:57" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>43</v>
       </c>
@@ -9169,50 +8587,8 @@
         <f t="shared" si="2"/>
         <v>1.3129303993080648</v>
       </c>
-      <c r="AH15">
-        <v>2.6554950000000002</v>
-      </c>
-      <c r="AJ15">
-        <v>2.745412</v>
-      </c>
-      <c r="AN15">
-        <v>6.828112</v>
-      </c>
-      <c r="AP15">
-        <v>6.2622799999999996</v>
-      </c>
-      <c r="AT15">
-        <v>12</v>
-      </c>
-      <c r="AU15" t="s">
-        <v>43</v>
-      </c>
-      <c r="AV15" t="s">
-        <v>40</v>
-      </c>
-      <c r="AW15" t="s">
-        <v>34</v>
-      </c>
-      <c r="AX15">
-        <v>7.4643920000000001</v>
-      </c>
-      <c r="BA15">
-        <v>12</v>
-      </c>
-      <c r="BB15" t="s">
-        <v>43</v>
-      </c>
-      <c r="BC15" t="s">
-        <v>40</v>
-      </c>
-      <c r="BD15" t="s">
-        <v>34</v>
-      </c>
-      <c r="BE15">
-        <v>2.670731</v>
-      </c>
-    </row>
-    <row r="16" spans="2:57" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>43</v>
       </c>
@@ -9236,50 +8612,8 @@
         <f t="shared" si="2"/>
         <v>1.4386323249000033</v>
       </c>
-      <c r="AH16">
-        <v>2.8705859999999999</v>
-      </c>
-      <c r="AJ16">
-        <v>2.8493110000000001</v>
-      </c>
-      <c r="AN16">
-        <v>6.919009</v>
-      </c>
-      <c r="AP16">
-        <v>6.3861290000000004</v>
-      </c>
-      <c r="AT16">
-        <v>13</v>
-      </c>
-      <c r="AU16" t="s">
-        <v>43</v>
-      </c>
-      <c r="AV16" t="s">
-        <v>40</v>
-      </c>
-      <c r="AW16" t="s">
-        <v>37</v>
-      </c>
-      <c r="AX16">
-        <v>7.6236660000000001</v>
-      </c>
-      <c r="BA16">
-        <v>13</v>
-      </c>
-      <c r="BB16" t="s">
-        <v>43</v>
-      </c>
-      <c r="BC16" t="s">
-        <v>40</v>
-      </c>
-      <c r="BD16" t="s">
-        <v>37</v>
-      </c>
-      <c r="BE16">
-        <v>3.1026220000000002</v>
-      </c>
-    </row>
-    <row r="17" spans="2:57" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>43</v>
       </c>
@@ -9303,38 +8637,8 @@
         <f t="shared" si="2"/>
         <v>1.5865902706005601</v>
       </c>
-      <c r="AT17">
-        <v>14</v>
-      </c>
-      <c r="AU17" t="s">
-        <v>43</v>
-      </c>
-      <c r="AV17" t="s">
-        <v>40</v>
-      </c>
-      <c r="AW17" t="s">
-        <v>38</v>
-      </c>
-      <c r="AX17">
-        <v>6.9179539999999999</v>
-      </c>
-      <c r="BA17">
-        <v>14</v>
-      </c>
-      <c r="BB17" t="s">
-        <v>43</v>
-      </c>
-      <c r="BC17" t="s">
-        <v>40</v>
-      </c>
-      <c r="BD17" t="s">
-        <v>38</v>
-      </c>
-      <c r="BE17">
-        <v>2.6562060000000001</v>
-      </c>
-    </row>
-    <row r="18" spans="2:57" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>44</v>
       </c>
@@ -9363,38 +8667,8 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AT18">
-        <v>15</v>
-      </c>
-      <c r="AU18" t="s">
-        <v>43</v>
-      </c>
-      <c r="AV18" t="s">
-        <v>40</v>
-      </c>
-      <c r="AW18" t="s">
-        <v>39</v>
-      </c>
-      <c r="AX18">
-        <v>6.8632220000000004</v>
-      </c>
-      <c r="BA18">
-        <v>15</v>
-      </c>
-      <c r="BB18" t="s">
-        <v>43</v>
-      </c>
-      <c r="BC18" t="s">
-        <v>40</v>
-      </c>
-      <c r="BD18" t="s">
-        <v>39</v>
-      </c>
-      <c r="BE18">
-        <v>2.774289</v>
-      </c>
-    </row>
-    <row r="19" spans="2:57" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>44</v>
       </c>
@@ -9419,38 +8693,8 @@
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="AT19">
-        <v>16</v>
-      </c>
-      <c r="AU19" t="s">
-        <v>44</v>
-      </c>
-      <c r="AV19" t="s">
-        <v>33</v>
-      </c>
-      <c r="AW19" t="s">
-        <v>34</v>
-      </c>
-      <c r="AX19">
-        <v>6.9033720000000001</v>
-      </c>
-      <c r="BA19">
-        <v>16</v>
-      </c>
-      <c r="BB19" t="s">
-        <v>44</v>
-      </c>
-      <c r="BC19" t="s">
-        <v>33</v>
-      </c>
-      <c r="BD19" t="s">
-        <v>34</v>
-      </c>
-      <c r="BE19">
-        <v>3.190118</v>
-      </c>
-    </row>
-    <row r="20" spans="2:57" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>44</v>
       </c>
@@ -9467,38 +8711,8 @@
         <v>9.5206529999999994</v>
       </c>
       <c r="H20" s="2"/>
-      <c r="AT20">
-        <v>17</v>
-      </c>
-      <c r="AU20" t="s">
-        <v>44</v>
-      </c>
-      <c r="AV20" t="s">
-        <v>33</v>
-      </c>
-      <c r="AW20" t="s">
-        <v>37</v>
-      </c>
-      <c r="AX20">
-        <v>6.647322</v>
-      </c>
-      <c r="BA20">
-        <v>17</v>
-      </c>
-      <c r="BB20" t="s">
-        <v>44</v>
-      </c>
-      <c r="BC20" t="s">
-        <v>33</v>
-      </c>
-      <c r="BD20" t="s">
-        <v>37</v>
-      </c>
-      <c r="BE20">
-        <v>3.1468889999999998</v>
-      </c>
-    </row>
-    <row r="21" spans="2:57" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>44</v>
       </c>
@@ -9515,38 +8729,8 @@
         <v>9.5206529999999994</v>
       </c>
       <c r="H21" s="2"/>
-      <c r="AT21">
-        <v>18</v>
-      </c>
-      <c r="AU21" t="s">
-        <v>44</v>
-      </c>
-      <c r="AV21" t="s">
-        <v>33</v>
-      </c>
-      <c r="AW21" t="s">
-        <v>38</v>
-      </c>
-      <c r="AX21">
-        <v>6.3015169999999996</v>
-      </c>
-      <c r="BA21">
-        <v>18</v>
-      </c>
-      <c r="BB21" t="s">
-        <v>44</v>
-      </c>
-      <c r="BC21" t="s">
-        <v>33</v>
-      </c>
-      <c r="BD21" t="s">
-        <v>38</v>
-      </c>
-      <c r="BE21">
-        <v>3.2110289999999999</v>
-      </c>
-    </row>
-    <row r="22" spans="2:57" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>44</v>
       </c>
@@ -9567,38 +8751,8 @@
         <v>9.8293160000000004</v>
       </c>
       <c r="H22" s="2"/>
-      <c r="AT22">
-        <v>19</v>
-      </c>
-      <c r="AU22" t="s">
-        <v>44</v>
-      </c>
-      <c r="AV22" t="s">
-        <v>33</v>
-      </c>
-      <c r="AW22" t="s">
-        <v>39</v>
-      </c>
-      <c r="AX22">
-        <v>6.898752</v>
-      </c>
-      <c r="BA22">
-        <v>19</v>
-      </c>
-      <c r="BB22" t="s">
-        <v>44</v>
-      </c>
-      <c r="BC22" t="s">
-        <v>33</v>
-      </c>
-      <c r="BD22" t="s">
-        <v>39</v>
-      </c>
-      <c r="BE22">
-        <v>3.5255000000000001</v>
-      </c>
-    </row>
-    <row r="23" spans="2:57" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>44</v>
       </c>
@@ -9615,38 +8769,8 @@
         <v>9.8293160000000004</v>
       </c>
       <c r="H23" s="2"/>
-      <c r="AT23">
-        <v>20</v>
-      </c>
-      <c r="AU23" t="s">
-        <v>44</v>
-      </c>
-      <c r="AV23" t="s">
-        <v>40</v>
-      </c>
-      <c r="AW23" t="s">
-        <v>34</v>
-      </c>
-      <c r="AX23">
-        <v>7.3225720000000001</v>
-      </c>
-      <c r="BA23">
-        <v>20</v>
-      </c>
-      <c r="BB23" t="s">
-        <v>44</v>
-      </c>
-      <c r="BC23" t="s">
-        <v>40</v>
-      </c>
-      <c r="BD23" t="s">
-        <v>34</v>
-      </c>
-      <c r="BE23">
-        <v>3.3469850000000001</v>
-      </c>
-    </row>
-    <row r="24" spans="2:57" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>44</v>
       </c>
@@ -9663,38 +8787,8 @@
         <v>9.8293160000000004</v>
       </c>
       <c r="H24" s="2"/>
-      <c r="AT24">
-        <v>21</v>
-      </c>
-      <c r="AU24" t="s">
-        <v>44</v>
-      </c>
-      <c r="AV24" t="s">
-        <v>40</v>
-      </c>
-      <c r="AW24" t="s">
-        <v>37</v>
-      </c>
-      <c r="AX24">
-        <v>7.7138470000000003</v>
-      </c>
-      <c r="BA24">
-        <v>21</v>
-      </c>
-      <c r="BB24" t="s">
-        <v>44</v>
-      </c>
-      <c r="BC24" t="s">
-        <v>40</v>
-      </c>
-      <c r="BD24" t="s">
-        <v>37</v>
-      </c>
-      <c r="BE24">
-        <v>3.0652469999999998</v>
-      </c>
-    </row>
-    <row r="25" spans="2:57" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>44</v>
       </c>
@@ -9711,38 +8805,8 @@
         <v>9.8293160000000004</v>
       </c>
       <c r="H25" s="2"/>
-      <c r="AT25">
-        <v>22</v>
-      </c>
-      <c r="AU25" t="s">
-        <v>44</v>
-      </c>
-      <c r="AV25" t="s">
-        <v>40</v>
-      </c>
-      <c r="AW25" t="s">
-        <v>38</v>
-      </c>
-      <c r="AX25">
-        <v>7.5333889999999997</v>
-      </c>
-      <c r="BA25">
-        <v>22</v>
-      </c>
-      <c r="BB25" t="s">
-        <v>44</v>
-      </c>
-      <c r="BC25" t="s">
-        <v>40</v>
-      </c>
-      <c r="BD25" t="s">
-        <v>38</v>
-      </c>
-      <c r="BE25">
-        <v>3.0850390000000001</v>
-      </c>
-    </row>
-    <row r="26" spans="2:57" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>45</v>
       </c>
@@ -9760,38 +8824,8 @@
         <v>9.1254899999999992</v>
       </c>
       <c r="H26" s="2"/>
-      <c r="AT26">
-        <v>23</v>
-      </c>
-      <c r="AU26" t="s">
-        <v>44</v>
-      </c>
-      <c r="AV26" t="s">
-        <v>40</v>
-      </c>
-      <c r="AW26" t="s">
-        <v>39</v>
-      </c>
-      <c r="AX26">
-        <v>7.8034150000000002</v>
-      </c>
-      <c r="BA26">
-        <v>23</v>
-      </c>
-      <c r="BB26" t="s">
-        <v>44</v>
-      </c>
-      <c r="BC26" t="s">
-        <v>40</v>
-      </c>
-      <c r="BD26" t="s">
-        <v>39</v>
-      </c>
-      <c r="BE26">
-        <v>3.1780020000000002</v>
-      </c>
-    </row>
-    <row r="27" spans="2:57" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>45</v>
       </c>
@@ -9805,38 +8839,8 @@
         <v>9.1254899999999992</v>
       </c>
       <c r="H27" s="2"/>
-      <c r="AT27">
-        <v>24</v>
-      </c>
-      <c r="AU27" t="s">
-        <v>45</v>
-      </c>
-      <c r="AV27" t="s">
-        <v>33</v>
-      </c>
-      <c r="AW27" t="s">
-        <v>34</v>
-      </c>
-      <c r="AX27">
-        <v>6.1153700000000004</v>
-      </c>
-      <c r="BA27">
-        <v>24</v>
-      </c>
-      <c r="BB27" t="s">
-        <v>45</v>
-      </c>
-      <c r="BC27" t="s">
-        <v>33</v>
-      </c>
-      <c r="BD27" t="s">
-        <v>34</v>
-      </c>
-      <c r="BE27">
-        <v>2.9394070000000001</v>
-      </c>
-    </row>
-    <row r="28" spans="2:57" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>45</v>
       </c>
@@ -9850,38 +8854,8 @@
         <v>9.1254899999999992</v>
       </c>
       <c r="H28" s="2"/>
-      <c r="AT28">
-        <v>25</v>
-      </c>
-      <c r="AU28" t="s">
-        <v>45</v>
-      </c>
-      <c r="AV28" t="s">
-        <v>33</v>
-      </c>
-      <c r="AW28" t="s">
-        <v>37</v>
-      </c>
-      <c r="AX28">
-        <v>5.5948729999999998</v>
-      </c>
-      <c r="BA28">
-        <v>25</v>
-      </c>
-      <c r="BB28" t="s">
-        <v>45</v>
-      </c>
-      <c r="BC28" t="s">
-        <v>33</v>
-      </c>
-      <c r="BD28" t="s">
-        <v>37</v>
-      </c>
-      <c r="BE28">
-        <v>2.7081900000000001</v>
-      </c>
-    </row>
-    <row r="29" spans="2:57" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>45</v>
       </c>
@@ -9895,38 +8869,8 @@
         <v>9.1254899999999992</v>
       </c>
       <c r="H29" s="2"/>
-      <c r="AT29">
-        <v>26</v>
-      </c>
-      <c r="AU29" t="s">
-        <v>45</v>
-      </c>
-      <c r="AV29" t="s">
-        <v>33</v>
-      </c>
-      <c r="AW29" t="s">
-        <v>38</v>
-      </c>
-      <c r="AX29">
-        <v>6.2622799999999996</v>
-      </c>
-      <c r="BA29">
-        <v>26</v>
-      </c>
-      <c r="BB29" t="s">
-        <v>45</v>
-      </c>
-      <c r="BC29" t="s">
-        <v>33</v>
-      </c>
-      <c r="BD29" t="s">
-        <v>38</v>
-      </c>
-      <c r="BE29">
-        <v>2.745412</v>
-      </c>
-    </row>
-    <row r="30" spans="2:57" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>45</v>
       </c>
@@ -9944,38 +8888,8 @@
         <v>9.0093949999999996</v>
       </c>
       <c r="H30" s="2"/>
-      <c r="AT30">
-        <v>27</v>
-      </c>
-      <c r="AU30" t="s">
-        <v>45</v>
-      </c>
-      <c r="AV30" t="s">
-        <v>33</v>
-      </c>
-      <c r="AW30" t="s">
-        <v>39</v>
-      </c>
-      <c r="AX30">
-        <v>6.3861290000000004</v>
-      </c>
-      <c r="BA30">
-        <v>27</v>
-      </c>
-      <c r="BB30" t="s">
-        <v>45</v>
-      </c>
-      <c r="BC30" t="s">
-        <v>33</v>
-      </c>
-      <c r="BD30" t="s">
-        <v>39</v>
-      </c>
-      <c r="BE30">
-        <v>2.8493110000000001</v>
-      </c>
-    </row>
-    <row r="31" spans="2:57" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>45</v>
       </c>
@@ -9989,38 +8903,8 @@
         <v>9.0093949999999996</v>
       </c>
       <c r="H31" s="2"/>
-      <c r="AT31">
-        <v>28</v>
-      </c>
-      <c r="AU31" t="s">
-        <v>45</v>
-      </c>
-      <c r="AV31" t="s">
-        <v>40</v>
-      </c>
-      <c r="AW31" t="s">
-        <v>34</v>
-      </c>
-      <c r="AX31">
-        <v>8.0594289999999997</v>
-      </c>
-      <c r="BA31">
-        <v>28</v>
-      </c>
-      <c r="BB31" t="s">
-        <v>45</v>
-      </c>
-      <c r="BC31" t="s">
-        <v>40</v>
-      </c>
-      <c r="BD31" t="s">
-        <v>34</v>
-      </c>
-      <c r="BE31">
-        <v>4.6571119999999997</v>
-      </c>
-    </row>
-    <row r="32" spans="2:57" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>45</v>
       </c>
@@ -10034,38 +8918,8 @@
         <v>9.0093949999999996</v>
       </c>
       <c r="H32" s="2"/>
-      <c r="AT32">
-        <v>29</v>
-      </c>
-      <c r="AU32" t="s">
-        <v>45</v>
-      </c>
-      <c r="AV32" t="s">
-        <v>40</v>
-      </c>
-      <c r="AW32" t="s">
-        <v>37</v>
-      </c>
-      <c r="AX32">
-        <v>6.5402509999999996</v>
-      </c>
-      <c r="BA32">
-        <v>29</v>
-      </c>
-      <c r="BB32" t="s">
-        <v>45</v>
-      </c>
-      <c r="BC32" t="s">
-        <v>40</v>
-      </c>
-      <c r="BD32" t="s">
-        <v>37</v>
-      </c>
-      <c r="BE32">
-        <v>2.8593359999999999</v>
-      </c>
-    </row>
-    <row r="33" spans="2:57" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>45</v>
       </c>
@@ -10079,68 +8933,6 @@
         <v>9.0093949999999996</v>
       </c>
       <c r="H33" s="2"/>
-      <c r="AT33">
-        <v>30</v>
-      </c>
-      <c r="AU33" t="s">
-        <v>45</v>
-      </c>
-      <c r="AV33" t="s">
-        <v>40</v>
-      </c>
-      <c r="AW33" t="s">
-        <v>38</v>
-      </c>
-      <c r="AX33">
-        <v>6.828112</v>
-      </c>
-      <c r="BA33">
-        <v>30</v>
-      </c>
-      <c r="BB33" t="s">
-        <v>45</v>
-      </c>
-      <c r="BC33" t="s">
-        <v>40</v>
-      </c>
-      <c r="BD33" t="s">
-        <v>38</v>
-      </c>
-      <c r="BE33">
-        <v>2.6554950000000002</v>
-      </c>
-    </row>
-    <row r="34" spans="2:57" x14ac:dyDescent="0.25">
-      <c r="AT34">
-        <v>31</v>
-      </c>
-      <c r="AU34" t="s">
-        <v>45</v>
-      </c>
-      <c r="AV34" t="s">
-        <v>40</v>
-      </c>
-      <c r="AW34" t="s">
-        <v>39</v>
-      </c>
-      <c r="AX34">
-        <v>6.919009</v>
-      </c>
-      <c r="BA34">
-        <v>31</v>
-      </c>
-      <c r="BB34" t="s">
-        <v>45</v>
-      </c>
-      <c r="BC34" t="s">
-        <v>40</v>
-      </c>
-      <c r="BD34" t="s">
-        <v>39</v>
-      </c>
-      <c r="BE34">
-        <v>2.8705859999999999</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -10357,10 +9149,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:T57"/>
+  <dimension ref="A1:T76"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42:E57"/>
+    <sheetView topLeftCell="A28" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
+      <selection activeCell="P43" sqref="P43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12036,6 +10828,9 @@
       <c r="F41" t="s">
         <v>19</v>
       </c>
+      <c r="K41" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42">
@@ -12056,6 +10851,18 @@
       <c r="F42">
         <v>8.9729109999999999</v>
       </c>
+      <c r="L42" t="s">
+        <v>14</v>
+      </c>
+      <c r="M42" t="s">
+        <v>15</v>
+      </c>
+      <c r="N42" t="s">
+        <v>16</v>
+      </c>
+      <c r="O42" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43">
@@ -12076,6 +10883,21 @@
       <c r="F43">
         <v>8.9729109999999999</v>
       </c>
+      <c r="K43">
+        <v>0</v>
+      </c>
+      <c r="L43" t="s">
+        <v>43</v>
+      </c>
+      <c r="M43" t="s">
+        <v>33</v>
+      </c>
+      <c r="N43" t="s">
+        <v>34</v>
+      </c>
+      <c r="O43">
+        <v>2.8224860000000001</v>
+      </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44">
@@ -12096,6 +10918,21 @@
       <c r="F44">
         <v>8.9729109999999999</v>
       </c>
+      <c r="K44">
+        <v>1</v>
+      </c>
+      <c r="L44" t="s">
+        <v>43</v>
+      </c>
+      <c r="M44" t="s">
+        <v>33</v>
+      </c>
+      <c r="N44" t="s">
+        <v>37</v>
+      </c>
+      <c r="O44">
+        <v>2.7806150000000001</v>
+      </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45">
@@ -12116,6 +10953,21 @@
       <c r="F45">
         <v>8.9729109999999999</v>
       </c>
+      <c r="K45">
+        <v>2</v>
+      </c>
+      <c r="L45" t="s">
+        <v>43</v>
+      </c>
+      <c r="M45" t="s">
+        <v>33</v>
+      </c>
+      <c r="N45" t="s">
+        <v>38</v>
+      </c>
+      <c r="O45">
+        <v>2.5526460000000002</v>
+      </c>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46">
@@ -12136,6 +10988,21 @@
       <c r="F46">
         <v>9.3905689999999993</v>
       </c>
+      <c r="K46">
+        <v>3</v>
+      </c>
+      <c r="L46" t="s">
+        <v>43</v>
+      </c>
+      <c r="M46" t="s">
+        <v>33</v>
+      </c>
+      <c r="N46" t="s">
+        <v>39</v>
+      </c>
+      <c r="O46">
+        <v>2.8426930000000001</v>
+      </c>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47">
@@ -12156,6 +11023,21 @@
       <c r="F47">
         <v>9.3905689999999993</v>
       </c>
+      <c r="K47">
+        <v>4</v>
+      </c>
+      <c r="L47" t="s">
+        <v>43</v>
+      </c>
+      <c r="M47" t="s">
+        <v>40</v>
+      </c>
+      <c r="N47" t="s">
+        <v>34</v>
+      </c>
+      <c r="O47">
+        <v>2.670731</v>
+      </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48">
@@ -12176,8 +11058,23 @@
       <c r="F48">
         <v>9.3905689999999993</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K48">
+        <v>5</v>
+      </c>
+      <c r="L48" t="s">
+        <v>43</v>
+      </c>
+      <c r="M48" t="s">
+        <v>40</v>
+      </c>
+      <c r="N48" t="s">
+        <v>37</v>
+      </c>
+      <c r="O48">
+        <v>3.1026220000000002</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>532</v>
       </c>
@@ -12196,8 +11093,23 @@
       <c r="F49">
         <v>9.3905689999999993</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K49">
+        <v>6</v>
+      </c>
+      <c r="L49" t="s">
+        <v>43</v>
+      </c>
+      <c r="M49" t="s">
+        <v>40</v>
+      </c>
+      <c r="N49" t="s">
+        <v>38</v>
+      </c>
+      <c r="O49">
+        <v>2.6562060000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>545</v>
       </c>
@@ -12216,8 +11128,23 @@
       <c r="F50">
         <v>9.5206529999999994</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K50">
+        <v>7</v>
+      </c>
+      <c r="L50" t="s">
+        <v>43</v>
+      </c>
+      <c r="M50" t="s">
+        <v>40</v>
+      </c>
+      <c r="N50" t="s">
+        <v>39</v>
+      </c>
+      <c r="O50">
+        <v>2.774289</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>546</v>
       </c>
@@ -12236,8 +11163,23 @@
       <c r="F51">
         <v>9.5206529999999994</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K51">
+        <v>8</v>
+      </c>
+      <c r="L51" t="s">
+        <v>44</v>
+      </c>
+      <c r="M51" t="s">
+        <v>33</v>
+      </c>
+      <c r="N51" t="s">
+        <v>34</v>
+      </c>
+      <c r="O51">
+        <v>3.190118</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>547</v>
       </c>
@@ -12256,8 +11198,23 @@
       <c r="F52">
         <v>9.5206529999999994</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K52">
+        <v>9</v>
+      </c>
+      <c r="L52" t="s">
+        <v>44</v>
+      </c>
+      <c r="M52" t="s">
+        <v>33</v>
+      </c>
+      <c r="N52" t="s">
+        <v>37</v>
+      </c>
+      <c r="O52">
+        <v>3.1468889999999998</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>548</v>
       </c>
@@ -12276,8 +11233,23 @@
       <c r="F53">
         <v>9.5206529999999994</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K53">
+        <v>10</v>
+      </c>
+      <c r="L53" t="s">
+        <v>44</v>
+      </c>
+      <c r="M53" t="s">
+        <v>33</v>
+      </c>
+      <c r="N53" t="s">
+        <v>38</v>
+      </c>
+      <c r="O53">
+        <v>3.2110289999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>561</v>
       </c>
@@ -12296,8 +11268,23 @@
       <c r="F54">
         <v>9.8293160000000004</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K54">
+        <v>11</v>
+      </c>
+      <c r="L54" t="s">
+        <v>44</v>
+      </c>
+      <c r="M54" t="s">
+        <v>33</v>
+      </c>
+      <c r="N54" t="s">
+        <v>39</v>
+      </c>
+      <c r="O54">
+        <v>3.5255000000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>562</v>
       </c>
@@ -12316,8 +11303,23 @@
       <c r="F55">
         <v>9.8293160000000004</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K55">
+        <v>12</v>
+      </c>
+      <c r="L55" t="s">
+        <v>44</v>
+      </c>
+      <c r="M55" t="s">
+        <v>40</v>
+      </c>
+      <c r="N55" t="s">
+        <v>34</v>
+      </c>
+      <c r="O55">
+        <v>3.3469850000000001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>563</v>
       </c>
@@ -12336,8 +11338,23 @@
       <c r="F56">
         <v>9.8293160000000004</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K56">
+        <v>13</v>
+      </c>
+      <c r="L56" t="s">
+        <v>44</v>
+      </c>
+      <c r="M56" t="s">
+        <v>40</v>
+      </c>
+      <c r="N56" t="s">
+        <v>37</v>
+      </c>
+      <c r="O56">
+        <v>3.0652469999999998</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>564</v>
       </c>
@@ -12355,6 +11372,329 @@
       </c>
       <c r="F57">
         <v>9.8293160000000004</v>
+      </c>
+      <c r="K57">
+        <v>14</v>
+      </c>
+      <c r="L57" t="s">
+        <v>44</v>
+      </c>
+      <c r="M57" t="s">
+        <v>40</v>
+      </c>
+      <c r="N57" t="s">
+        <v>38</v>
+      </c>
+      <c r="O57">
+        <v>3.0850390000000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K58">
+        <v>15</v>
+      </c>
+      <c r="L58" t="s">
+        <v>44</v>
+      </c>
+      <c r="M58" t="s">
+        <v>40</v>
+      </c>
+      <c r="N58" t="s">
+        <v>39</v>
+      </c>
+      <c r="O58">
+        <v>3.1780020000000002</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K59" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L60" t="s">
+        <v>14</v>
+      </c>
+      <c r="M60" t="s">
+        <v>15</v>
+      </c>
+      <c r="N60" t="s">
+        <v>16</v>
+      </c>
+      <c r="O60" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K61">
+        <v>0</v>
+      </c>
+      <c r="L61" t="s">
+        <v>43</v>
+      </c>
+      <c r="M61" t="s">
+        <v>33</v>
+      </c>
+      <c r="N61" t="s">
+        <v>34</v>
+      </c>
+      <c r="O61">
+        <v>6.6376109999999997</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K62">
+        <v>1</v>
+      </c>
+      <c r="L62" t="s">
+        <v>43</v>
+      </c>
+      <c r="M62" t="s">
+        <v>33</v>
+      </c>
+      <c r="N62" t="s">
+        <v>37</v>
+      </c>
+      <c r="O62">
+        <v>5.9639850000000001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K63">
+        <v>2</v>
+      </c>
+      <c r="L63" t="s">
+        <v>43</v>
+      </c>
+      <c r="M63" t="s">
+        <v>33</v>
+      </c>
+      <c r="N63" t="s">
+        <v>38</v>
+      </c>
+      <c r="O63">
+        <v>6.6552610000000003</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K64">
+        <v>3</v>
+      </c>
+      <c r="L64" t="s">
+        <v>43</v>
+      </c>
+      <c r="M64" t="s">
+        <v>33</v>
+      </c>
+      <c r="N64" t="s">
+        <v>39</v>
+      </c>
+      <c r="O64">
+        <v>5.8253329999999997</v>
+      </c>
+    </row>
+    <row r="65" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K65">
+        <v>4</v>
+      </c>
+      <c r="L65" t="s">
+        <v>43</v>
+      </c>
+      <c r="M65" t="s">
+        <v>40</v>
+      </c>
+      <c r="N65" t="s">
+        <v>34</v>
+      </c>
+      <c r="O65">
+        <v>7.4643920000000001</v>
+      </c>
+    </row>
+    <row r="66" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K66">
+        <v>5</v>
+      </c>
+      <c r="L66" t="s">
+        <v>43</v>
+      </c>
+      <c r="M66" t="s">
+        <v>40</v>
+      </c>
+      <c r="N66" t="s">
+        <v>37</v>
+      </c>
+      <c r="O66">
+        <v>7.6236660000000001</v>
+      </c>
+    </row>
+    <row r="67" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K67">
+        <v>6</v>
+      </c>
+      <c r="L67" t="s">
+        <v>43</v>
+      </c>
+      <c r="M67" t="s">
+        <v>40</v>
+      </c>
+      <c r="N67" t="s">
+        <v>38</v>
+      </c>
+      <c r="O67">
+        <v>6.9179539999999999</v>
+      </c>
+    </row>
+    <row r="68" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K68">
+        <v>7</v>
+      </c>
+      <c r="L68" t="s">
+        <v>43</v>
+      </c>
+      <c r="M68" t="s">
+        <v>40</v>
+      </c>
+      <c r="N68" t="s">
+        <v>39</v>
+      </c>
+      <c r="O68">
+        <v>6.8632220000000004</v>
+      </c>
+    </row>
+    <row r="69" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K69">
+        <v>8</v>
+      </c>
+      <c r="L69" t="s">
+        <v>44</v>
+      </c>
+      <c r="M69" t="s">
+        <v>33</v>
+      </c>
+      <c r="N69" t="s">
+        <v>34</v>
+      </c>
+      <c r="O69">
+        <v>6.9033720000000001</v>
+      </c>
+    </row>
+    <row r="70" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K70">
+        <v>9</v>
+      </c>
+      <c r="L70" t="s">
+        <v>44</v>
+      </c>
+      <c r="M70" t="s">
+        <v>33</v>
+      </c>
+      <c r="N70" t="s">
+        <v>37</v>
+      </c>
+      <c r="O70">
+        <v>6.647322</v>
+      </c>
+    </row>
+    <row r="71" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K71">
+        <v>10</v>
+      </c>
+      <c r="L71" t="s">
+        <v>44</v>
+      </c>
+      <c r="M71" t="s">
+        <v>33</v>
+      </c>
+      <c r="N71" t="s">
+        <v>38</v>
+      </c>
+      <c r="O71">
+        <v>6.3015169999999996</v>
+      </c>
+    </row>
+    <row r="72" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K72">
+        <v>11</v>
+      </c>
+      <c r="L72" t="s">
+        <v>44</v>
+      </c>
+      <c r="M72" t="s">
+        <v>33</v>
+      </c>
+      <c r="N72" t="s">
+        <v>39</v>
+      </c>
+      <c r="O72">
+        <v>6.898752</v>
+      </c>
+    </row>
+    <row r="73" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K73">
+        <v>12</v>
+      </c>
+      <c r="L73" t="s">
+        <v>44</v>
+      </c>
+      <c r="M73" t="s">
+        <v>40</v>
+      </c>
+      <c r="N73" t="s">
+        <v>34</v>
+      </c>
+      <c r="O73">
+        <v>7.3225720000000001</v>
+      </c>
+    </row>
+    <row r="74" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K74">
+        <v>13</v>
+      </c>
+      <c r="L74" t="s">
+        <v>44</v>
+      </c>
+      <c r="M74" t="s">
+        <v>40</v>
+      </c>
+      <c r="N74" t="s">
+        <v>37</v>
+      </c>
+      <c r="O74">
+        <v>7.7138470000000003</v>
+      </c>
+    </row>
+    <row r="75" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K75">
+        <v>14</v>
+      </c>
+      <c r="L75" t="s">
+        <v>44</v>
+      </c>
+      <c r="M75" t="s">
+        <v>40</v>
+      </c>
+      <c r="N75" t="s">
+        <v>38</v>
+      </c>
+      <c r="O75">
+        <v>7.5333889999999997</v>
+      </c>
+    </row>
+    <row r="76" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K76">
+        <v>15</v>
+      </c>
+      <c r="L76" t="s">
+        <v>44</v>
+      </c>
+      <c r="M76" t="s">
+        <v>40</v>
+      </c>
+      <c r="N76" t="s">
+        <v>39</v>
+      </c>
+      <c r="O76">
+        <v>7.8034150000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating some figures to push towards phd lunch meeting
</commit_message>
<xml_diff>
--- a/metaboliccostcomparisons.xlsx
+++ b/metaboliccostcomparisons.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\code\repos\Stanford\delplab\projects\muscleModel\muscleEnergyModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655AE7FC-58FB-4EFC-8682-276515398B80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C148439C-E651-49F7-A899-49DB7DE3EA6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,15 +31,12 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="99">
   <si>
     <t>t-Test: Paired Two Sample for Means</t>
   </si>
@@ -301,11 +298,50 @@
   <si>
     <t>'mechanical_work_rate_soleus_r_TOTAL'</t>
   </si>
+  <si>
+    <t>swing exo</t>
+  </si>
+  <si>
+    <t>swing natural</t>
+  </si>
+  <si>
+    <t>stance exo</t>
+  </si>
+  <si>
+    <t>stance natural</t>
+  </si>
+  <si>
+    <t>subject avg</t>
+  </si>
+  <si>
+    <t>Absolute difference experiment</t>
+  </si>
+  <si>
+    <t>absolute difference simulation with basal</t>
+  </si>
+  <si>
+    <t>absolute differnce without basal</t>
+  </si>
+  <si>
+    <t>delta</t>
+  </si>
+  <si>
+    <t>delta percent whole</t>
+  </si>
+  <si>
+    <t>delta perc</t>
+  </si>
+  <si>
+    <t>STDEV</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -449,7 +485,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -468,6 +504,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -541,6 +578,10 @@
       <rgbColor rgb="00333399"/>
       <rgbColor rgb="00333333"/>
     </indexedColors>
+    <mruColors>
+      <color rgb="FFFF8B8B"/>
+      <color rgb="FFFF8181"/>
+    </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1205,6 +1246,978 @@
       <a:round/>
     </a:ln>
   </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="4000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="4000"/>
+              <a:t>Metabolic Savings with Exotendon</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="4000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Swing Natural</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>(alldata_1step!$AU$4,alldata_1step!$AU$8)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>9.0008547311491521E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>5.5662879589290733E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>(alldata_1step!$AU$4,alldata_1step!$AU$8)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>9.0008547311491521E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>5.5662879589290733E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:val>
+            <c:numRef>
+              <c:f>(alldata_1step!$AU$3,alldata_1step!$AU$7)</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>2.8009620000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.1688182500000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-591C-44B3-A765-44177E63EE17}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Swing Exo</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>(alldata_1step!$AL$4,alldata_1step!$AL$8)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>5.7950131355545671E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>7.5118587605698534E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>(alldata_1step!$AL$4,alldata_1step!$AL$8)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>5.7950131355545671E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>7.5118587605698534E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:val>
+            <c:numRef>
+              <c:f>(alldata_1step!$AL$3,alldata_1step!$AL$7)</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>2.7496100000000006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.2683840000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5727-4881-9B43-FFFBEDB1D735}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Stance Natural </c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="C00000"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>(alldata_1step!$BM$4,alldata_1step!$BM$8)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>0.16605101624406729</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>9.2047158499987847E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>(alldata_1step!$BM$4,alldata_1step!$BM$8)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>0.16605101624406729</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>9.2047158499987847E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:val>
+            <c:numRef>
+              <c:f>(alldata_1step!$BM$3,alldata_1step!$BM$7)</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>7.2173084999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.5933057500000007</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5727-4881-9B43-FFFBEDB1D735}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Stance Exo</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF8B8B"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>(alldata_1step!$BD$4,alldata_1step!$BD$8)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>0.18956143587419758</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.12293927464879519</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>(alldata_1step!$BD$4,alldata_1step!$BD$8)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>0.18956143587419758</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.12293927464879519</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:val>
+            <c:numRef>
+              <c:f>(alldata_1step!$BD$3,alldata_1step!$BD$7)</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>6.2705475000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.6877407499999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-5727-4881-9B43-FFFBEDB1D735}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="38660507"/>
+        <c:axId val="84186580"/>
+        <c:extLst/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="38660507"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="3200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="3200"/>
+                  <a:t>Subjects</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.51131700037308803"/>
+              <c:y val="0.83119792133321402"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="3200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="84186580"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="84186580"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="9"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="4000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="4000"/>
+                  <a:t>Metabolic Power [W/kg]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="4000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="3200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="38660507"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -4225,7 +5238,14 @@
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
-  <c:style val="2"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -4269,7 +5289,7 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="2"/>
           <c:order val="0"/>
           <c:tx>
             <c:v>Experimental</c:v>
@@ -4283,44 +5303,6 @@
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr wrap="square"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="1"/>
-            <c:separator>; </c:separator>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
           <c:cat>
             <c:strLit>
               <c:ptCount val="2"/>
@@ -4361,12 +5343,12 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-1898-4B2D-9731-ACA81D036281}"/>
+              <c16:uniqueId val="{00000005-591C-44B3-A765-44177E63EE17}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="3"/>
           <c:order val="1"/>
           <c:tx>
             <c:v>Simulation (w/o basal)</c:v>
@@ -4380,44 +5362,6 @@
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr wrap="square"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Calibri"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="1"/>
-            <c:separator>; </c:separator>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
           <c:cat>
             <c:strLit>
               <c:ptCount val="2"/>
@@ -4458,7 +5402,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-1898-4B2D-9731-ACA81D036281}"/>
+              <c16:uniqueId val="{00000006-591C-44B3-A765-44177E63EE17}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4474,6 +5418,174 @@
         <c:overlap val="-27"/>
         <c:axId val="38660507"/>
         <c:axId val="84186580"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:v>Experimental</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:srgbClr val="4472C4"/>
+                  </a:solidFill>
+                  <a:ln w="0">
+                    <a:noFill/>
+                  </a:ln>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr wrap="square"/>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                          <a:solidFill>
+                            <a:srgbClr val="000000"/>
+                          </a:solidFill>
+                          <a:latin typeface="Calibri"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="outEnd"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="0"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="1"/>
+                  <c:separator>; </c:separator>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>alldata_1step!$M$3:$M$4</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>alldata_1step!$M$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>-3.1402286791878598</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000002-591C-44B3-A765-44177E63EE17}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="3"/>
+                <c:tx>
+                  <c:v>Simulation (w/o basal)</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:srgbClr val="ED7D31"/>
+                  </a:solidFill>
+                  <a:ln w="0">
+                    <a:noFill/>
+                  </a:ln>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr wrap="square"/>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                          <a:solidFill>
+                            <a:srgbClr val="000000"/>
+                          </a:solidFill>
+                          <a:latin typeface="Calibri"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="outEnd"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="0"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="1"/>
+                  <c:separator>; </c:separator>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>alldata_1step!$Q$3:$Q$4</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>alldata_1step!$Q$4</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>-3.7297543833232742</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000004-591C-44B3-A765-44177E63EE17}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
       </c:barChart>
       <c:catAx>
         <c:axId val="38660507"/>
@@ -4995,6 +6107,1126 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-US" sz="4000" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="4000" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:rPr>
+              <a:t>Metabolic Savings with Exotendon</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Experimental</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="4472C4"/>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="2"/>
+              <c:pt idx="0">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>3</c:v>
+              </c:pt>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:autoCat val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>alldata_1step!$N$12:$N$15</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>alldata_1step!$N$13:$N$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>-0.41765799999999942</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.30866300000000102</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-591C-44B3-A765-44177E63EE17}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Simulation (w/o basal)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ED7D31"/>
+            </a:solidFill>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="2"/>
+              <c:pt idx="0">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>3</c:v>
+              </c:pt>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:autoCat val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>alldata_1step!$O$12:$O$15</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>alldata_1step!$O$13:$O$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>-0.75038875000000083</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.36883224999999875</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-591C-44B3-A765-44177E63EE17}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="38660507"/>
+        <c:axId val="84186580"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:v>Experimental</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:srgbClr val="4472C4"/>
+                  </a:solidFill>
+                  <a:ln w="0">
+                    <a:noFill/>
+                  </a:ln>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr wrap="square"/>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                          <a:solidFill>
+                            <a:srgbClr val="000000"/>
+                          </a:solidFill>
+                          <a:latin typeface="Calibri"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="outEnd"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="0"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="1"/>
+                  <c:separator>; </c:separator>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>alldata_1step!$N$12:$N$15</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>alldata_1step!$N$13:$N$14</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="2"/>
+                      <c:pt idx="0">
+                        <c:v>-0.41765799999999942</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>-0.30866300000000102</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000002-591C-44B3-A765-44177E63EE17}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="3"/>
+                <c:tx>
+                  <c:v>Simulation (w/o basal)</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:srgbClr val="ED7D31"/>
+                  </a:solidFill>
+                  <a:ln w="0">
+                    <a:noFill/>
+                  </a:ln>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr wrap="square"/>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="1000" b="0" strike="noStrike" spc="-1">
+                          <a:solidFill>
+                            <a:srgbClr val="000000"/>
+                          </a:solidFill>
+                          <a:latin typeface="Calibri"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="outEnd"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="0"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="1"/>
+                  <c:separator>; </c:separator>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:fullRef>
+                          <c15:sqref>alldata_1step!$P$12:$P$15</c15:sqref>
+                        </c15:fullRef>
+                        <c15:formulaRef>
+                          <c15:sqref>alldata_1step!$P$13:$P$14</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="2"/>
+                      <c:pt idx="0">
+                        <c:v>-0.75038875000000083</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>-0.36883224999999875</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000004-591C-44B3-A765-44177E63EE17}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="38660507"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr lang="en-US" sz="3600" b="0" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="3600" b="0" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Subjects</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.51131700037308803"/>
+              <c:y val="0.83119792133321402"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:ln w="9360">
+            <a:solidFill>
+              <a:srgbClr val="D9D9D9"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="3200" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="84186580"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="84186580"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9360">
+              <a:solidFill>
+                <a:srgbClr val="D9D9D9"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr lang="en-US" sz="3600" b="0" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="3600" b="0" strike="noStrike" spc="-1">
+                    <a:solidFill>
+                      <a:srgbClr val="595959"/>
+                    </a:solidFill>
+                    <a:latin typeface="Calibri"/>
+                  </a:rPr>
+                  <a:t>Change in Metabolic Power [W/kg]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="0">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="6480">
+            <a:noFill/>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="3200" b="0" strike="noStrike" spc="-1">
+                <a:solidFill>
+                  <a:srgbClr val="595959"/>
+                </a:solidFill>
+                <a:latin typeface="Calibri"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="38660507"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2400" b="0" strike="noStrike" spc="-1">
+              <a:solidFill>
+                <a:srgbClr val="595959"/>
+              </a:solidFill>
+              <a:latin typeface="Calibri"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="FFFFFF"/>
+    </a:solidFill>
+    <a:ln w="9360">
+      <a:solidFill>
+        <a:srgbClr val="D9D9D9"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
@@ -5220,16 +7452,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>455040</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>170088</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>544687</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>158882</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>40</xdr:col>
-      <xdr:colOff>68035</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>17007</xdr:rowOff>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>86767</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>5801</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5285,6 +7517,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>522276</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>158882</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>54</xdr:col>
+      <xdr:colOff>333297</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>5801</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{116E992A-80BD-46DF-9205-791C42424A64}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>55</xdr:col>
+      <xdr:colOff>495062</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>158882</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>71</xdr:col>
+      <xdr:colOff>360512</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>5801</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E35F509-C703-44D1-B5D8-DDD15800B635}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -8028,10 +10332,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="B1:Q33"/>
+  <dimension ref="B1:BN33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="67" zoomScaleNormal="65" workbookViewId="0">
-      <selection activeCell="AG1" sqref="AG1:AQ16"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="BN8" sqref="BN8:BN9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8052,9 +10356,13 @@
     <col min="15" max="15" width="29.85546875" customWidth="1"/>
     <col min="16" max="16" width="29.140625" customWidth="1"/>
     <col min="17" max="17" width="29.42578125" customWidth="1"/>
+    <col min="32" max="32" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>14</v>
       </c>
@@ -8103,8 +10411,38 @@
       <c r="Q1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="AF1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>95</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>97</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>32</v>
       </c>
@@ -8160,8 +10498,59 @@
         <f>(K2-K3)/K3*100</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="AH2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>14</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>15</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>16</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>53</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>14</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>15</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>16</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>32</v>
       </c>
@@ -8213,8 +10602,100 @@
         <f>(K4-K5)/(K5)*100</f>
         <v>-8.0372380116609783</v>
       </c>
-    </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="AG3">
+        <v>0</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AK3">
+        <v>2.8224860000000001</v>
+      </c>
+      <c r="AL3" s="16">
+        <f>AVERAGE(AK3:AK6)</f>
+        <v>2.7496100000000006</v>
+      </c>
+      <c r="AM3" s="16">
+        <f>AL3-AU3</f>
+        <v>-5.135199999999962E-2</v>
+      </c>
+      <c r="AN3">
+        <f>AM3/K5*100</f>
+        <v>-0.55001923519617146</v>
+      </c>
+      <c r="AP3">
+        <v>4</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AR3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AS3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AT3">
+        <v>2.670731</v>
+      </c>
+      <c r="AU3" s="16">
+        <f>AVERAGE(AT3:AT6)</f>
+        <v>2.8009620000000002</v>
+      </c>
+      <c r="AY3">
+        <v>0</v>
+      </c>
+      <c r="AZ3" t="s">
+        <v>43</v>
+      </c>
+      <c r="BA3" t="s">
+        <v>33</v>
+      </c>
+      <c r="BB3" t="s">
+        <v>34</v>
+      </c>
+      <c r="BC3">
+        <v>6.6376109999999997</v>
+      </c>
+      <c r="BD3" s="16">
+        <f>AVERAGE(BC3:BC6)</f>
+        <v>6.2705475000000002</v>
+      </c>
+      <c r="BE3" s="16">
+        <f>BD3-BM3</f>
+        <v>-0.94676099999999952</v>
+      </c>
+      <c r="BF3">
+        <f>BE3/K5*100</f>
+        <v>-10.140535152156996</v>
+      </c>
+      <c r="BH3">
+        <v>4</v>
+      </c>
+      <c r="BI3" t="s">
+        <v>43</v>
+      </c>
+      <c r="BJ3" t="s">
+        <v>40</v>
+      </c>
+      <c r="BK3" t="s">
+        <v>34</v>
+      </c>
+      <c r="BL3">
+        <v>7.4643920000000001</v>
+      </c>
+      <c r="BM3" s="16">
+        <f>AVERAGE(BL3:BL6)</f>
+        <v>7.2173084999999997</v>
+      </c>
+    </row>
+    <row r="4" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>32</v>
       </c>
@@ -8262,8 +10743,96 @@
         <f>(K6-K7)/K7*100</f>
         <v>-3.7297543833232742</v>
       </c>
-    </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="AG4">
+        <v>1</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK4">
+        <v>2.7806150000000001</v>
+      </c>
+      <c r="AL4">
+        <f>AL5/SQRT(COUNT(AK3:AK6))</f>
+        <v>5.7950131355545671E-2</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AP4">
+        <v>5</v>
+      </c>
+      <c r="AQ4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AS4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AT4">
+        <v>3.1026220000000002</v>
+      </c>
+      <c r="AU4">
+        <f>AU5/SQRT(COUNT(AT3:AT6))</f>
+        <v>9.0008547311491521E-2</v>
+      </c>
+      <c r="AV4" t="s">
+        <v>56</v>
+      </c>
+      <c r="AY4">
+        <v>1</v>
+      </c>
+      <c r="AZ4" t="s">
+        <v>43</v>
+      </c>
+      <c r="BA4" t="s">
+        <v>33</v>
+      </c>
+      <c r="BB4" t="s">
+        <v>37</v>
+      </c>
+      <c r="BC4">
+        <v>5.9639850000000001</v>
+      </c>
+      <c r="BD4">
+        <f>BD5/SQRT(COUNT(BC3:BC6))</f>
+        <v>0.18956143587419758</v>
+      </c>
+      <c r="BE4" t="s">
+        <v>56</v>
+      </c>
+      <c r="BH4">
+        <v>5</v>
+      </c>
+      <c r="BI4" t="s">
+        <v>43</v>
+      </c>
+      <c r="BJ4" t="s">
+        <v>40</v>
+      </c>
+      <c r="BK4" t="s">
+        <v>37</v>
+      </c>
+      <c r="BL4">
+        <v>7.6236660000000001</v>
+      </c>
+      <c r="BM4">
+        <f>BM5/SQRT(COUNT(BL3:BL6))</f>
+        <v>0.16605101624406729</v>
+      </c>
+      <c r="BN4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>32</v>
       </c>
@@ -8311,8 +10880,96 @@
         <f>(K8-K9)/K9*100</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="AG5">
+        <v>2</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>43</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>38</v>
+      </c>
+      <c r="AK5">
+        <v>2.5526460000000002</v>
+      </c>
+      <c r="AL5">
+        <f>_xlfn.STDEV.P(AK3:AK6)</f>
+        <v>0.11590026271109134</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>98</v>
+      </c>
+      <c r="AP5">
+        <v>6</v>
+      </c>
+      <c r="AQ5" t="s">
+        <v>43</v>
+      </c>
+      <c r="AR5" t="s">
+        <v>40</v>
+      </c>
+      <c r="AS5" t="s">
+        <v>38</v>
+      </c>
+      <c r="AT5">
+        <v>2.6562060000000001</v>
+      </c>
+      <c r="AU5">
+        <f>_xlfn.STDEV.P(AT3:AT6)</f>
+        <v>0.18001709462298304</v>
+      </c>
+      <c r="AV5" t="s">
+        <v>98</v>
+      </c>
+      <c r="AY5">
+        <v>2</v>
+      </c>
+      <c r="AZ5" t="s">
+        <v>43</v>
+      </c>
+      <c r="BA5" t="s">
+        <v>33</v>
+      </c>
+      <c r="BB5" t="s">
+        <v>38</v>
+      </c>
+      <c r="BC5">
+        <v>6.6552610000000003</v>
+      </c>
+      <c r="BD5">
+        <f>_xlfn.STDEV.P(BC3:BC6)</f>
+        <v>0.37912287174839515</v>
+      </c>
+      <c r="BE5" t="s">
+        <v>98</v>
+      </c>
+      <c r="BH5">
+        <v>6</v>
+      </c>
+      <c r="BI5" t="s">
+        <v>43</v>
+      </c>
+      <c r="BJ5" t="s">
+        <v>40</v>
+      </c>
+      <c r="BK5" t="s">
+        <v>38</v>
+      </c>
+      <c r="BL5">
+        <v>6.9179539999999999</v>
+      </c>
+      <c r="BM5">
+        <f>_xlfn.STDEV.P(BL3:BL6)</f>
+        <v>0.33210203248813458</v>
+      </c>
+      <c r="BN5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>32</v>
       </c>
@@ -8341,8 +10998,68 @@
         <f t="shared" si="0"/>
         <v>9.5200830000000014</v>
       </c>
-    </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="AG6">
+        <v>3</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>43</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>39</v>
+      </c>
+      <c r="AK6">
+        <v>2.8426930000000001</v>
+      </c>
+      <c r="AP6">
+        <v>7</v>
+      </c>
+      <c r="AQ6" t="s">
+        <v>43</v>
+      </c>
+      <c r="AR6" t="s">
+        <v>40</v>
+      </c>
+      <c r="AS6" t="s">
+        <v>39</v>
+      </c>
+      <c r="AT6">
+        <v>2.774289</v>
+      </c>
+      <c r="AY6">
+        <v>3</v>
+      </c>
+      <c r="AZ6" t="s">
+        <v>43</v>
+      </c>
+      <c r="BA6" t="s">
+        <v>33</v>
+      </c>
+      <c r="BB6" t="s">
+        <v>39</v>
+      </c>
+      <c r="BC6">
+        <v>5.8253329999999997</v>
+      </c>
+      <c r="BH6">
+        <v>7</v>
+      </c>
+      <c r="BI6" t="s">
+        <v>43</v>
+      </c>
+      <c r="BJ6" t="s">
+        <v>40</v>
+      </c>
+      <c r="BK6" t="s">
+        <v>39</v>
+      </c>
+      <c r="BL6">
+        <v>6.8632220000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>32</v>
       </c>
@@ -8367,8 +11084,100 @@
         <f t="shared" si="0"/>
         <v>9.8889152500000002</v>
       </c>
-    </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="AG7">
+        <v>8</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>34</v>
+      </c>
+      <c r="AK7">
+        <v>3.190118</v>
+      </c>
+      <c r="AL7" s="16">
+        <f>AVERAGE(AK7:AK10)</f>
+        <v>3.2683840000000002</v>
+      </c>
+      <c r="AM7" s="16">
+        <f>AL7-AU7</f>
+        <v>9.9565750000000008E-2</v>
+      </c>
+      <c r="AN7">
+        <f>AM7/K7*100</f>
+        <v>1.0068419789521406</v>
+      </c>
+      <c r="AP7">
+        <v>12</v>
+      </c>
+      <c r="AQ7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AR7" t="s">
+        <v>40</v>
+      </c>
+      <c r="AS7" t="s">
+        <v>34</v>
+      </c>
+      <c r="AT7">
+        <v>3.3469850000000001</v>
+      </c>
+      <c r="AU7" s="16">
+        <f>AVERAGE(AT7:AT10)</f>
+        <v>3.1688182500000002</v>
+      </c>
+      <c r="AY7">
+        <v>8</v>
+      </c>
+      <c r="AZ7" t="s">
+        <v>44</v>
+      </c>
+      <c r="BA7" t="s">
+        <v>33</v>
+      </c>
+      <c r="BB7" t="s">
+        <v>34</v>
+      </c>
+      <c r="BC7">
+        <v>6.9033720000000001</v>
+      </c>
+      <c r="BD7" s="16">
+        <f>AVERAGE(BC7:BC10)</f>
+        <v>6.6877407499999997</v>
+      </c>
+      <c r="BE7" s="16">
+        <f>BD7-BM7</f>
+        <v>-0.90556500000000106</v>
+      </c>
+      <c r="BF7">
+        <f>BE7/K7*100</f>
+        <v>-9.1573744653135858</v>
+      </c>
+      <c r="BH7">
+        <v>12</v>
+      </c>
+      <c r="BI7" t="s">
+        <v>44</v>
+      </c>
+      <c r="BJ7" t="s">
+        <v>40</v>
+      </c>
+      <c r="BK7" t="s">
+        <v>34</v>
+      </c>
+      <c r="BL7">
+        <v>7.3225720000000001</v>
+      </c>
+      <c r="BM7" s="16">
+        <f>AVERAGE(BL7:BL10)</f>
+        <v>7.5933057500000007</v>
+      </c>
+    </row>
+    <row r="8" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>32</v>
       </c>
@@ -8399,8 +11208,96 @@
       <c r="O8" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="AG8">
+        <v>9</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK8">
+        <v>3.1468889999999998</v>
+      </c>
+      <c r="AL8">
+        <f>AL9/SQRT(COUNT(AK7:AK10))</f>
+        <v>7.5118587605698534E-2</v>
+      </c>
+      <c r="AM8" t="s">
+        <v>56</v>
+      </c>
+      <c r="AP8">
+        <v>13</v>
+      </c>
+      <c r="AQ8" t="s">
+        <v>44</v>
+      </c>
+      <c r="AR8" t="s">
+        <v>40</v>
+      </c>
+      <c r="AS8" t="s">
+        <v>37</v>
+      </c>
+      <c r="AT8">
+        <v>3.0652469999999998</v>
+      </c>
+      <c r="AU8">
+        <f>AU9/SQRT(COUNT(AT7:AT10))</f>
+        <v>5.5662879589290733E-2</v>
+      </c>
+      <c r="AV8" t="s">
+        <v>56</v>
+      </c>
+      <c r="AY8">
+        <v>9</v>
+      </c>
+      <c r="AZ8" t="s">
+        <v>44</v>
+      </c>
+      <c r="BA8" t="s">
+        <v>33</v>
+      </c>
+      <c r="BB8" t="s">
+        <v>37</v>
+      </c>
+      <c r="BC8">
+        <v>6.647322</v>
+      </c>
+      <c r="BD8">
+        <f>BD9/SQRT(COUNT(BC7:BC10))</f>
+        <v>0.12293927464879519</v>
+      </c>
+      <c r="BE8" t="s">
+        <v>56</v>
+      </c>
+      <c r="BH8">
+        <v>13</v>
+      </c>
+      <c r="BI8" t="s">
+        <v>44</v>
+      </c>
+      <c r="BJ8" t="s">
+        <v>40</v>
+      </c>
+      <c r="BK8" t="s">
+        <v>37</v>
+      </c>
+      <c r="BL8">
+        <v>7.7138470000000003</v>
+      </c>
+      <c r="BM8">
+        <f>BM9/SQRT(COUNT(BL7:BL10))</f>
+        <v>9.2047158499987847E-2</v>
+      </c>
+      <c r="BN8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>32</v>
       </c>
@@ -8425,8 +11322,96 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="AG9">
+        <v>10</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>38</v>
+      </c>
+      <c r="AK9">
+        <v>3.2110289999999999</v>
+      </c>
+      <c r="AL9">
+        <f>_xlfn.STDEV.P(AK7:AK10)</f>
+        <v>0.15023717521139707</v>
+      </c>
+      <c r="AM9" t="s">
+        <v>98</v>
+      </c>
+      <c r="AP9">
+        <v>14</v>
+      </c>
+      <c r="AQ9" t="s">
+        <v>44</v>
+      </c>
+      <c r="AR9" t="s">
+        <v>40</v>
+      </c>
+      <c r="AS9" t="s">
+        <v>38</v>
+      </c>
+      <c r="AT9">
+        <v>3.0850390000000001</v>
+      </c>
+      <c r="AU9">
+        <f>_xlfn.STDEV.P(AT7:AT10)</f>
+        <v>0.11132575917858147</v>
+      </c>
+      <c r="AV9" t="s">
+        <v>98</v>
+      </c>
+      <c r="AY9">
+        <v>10</v>
+      </c>
+      <c r="AZ9" t="s">
+        <v>44</v>
+      </c>
+      <c r="BA9" t="s">
+        <v>33</v>
+      </c>
+      <c r="BB9" t="s">
+        <v>38</v>
+      </c>
+      <c r="BC9">
+        <v>6.3015169999999996</v>
+      </c>
+      <c r="BD9">
+        <f>_xlfn.STDEV.P(BC7:BC10)</f>
+        <v>0.24587854929759037</v>
+      </c>
+      <c r="BE9" t="s">
+        <v>98</v>
+      </c>
+      <c r="BH9">
+        <v>14</v>
+      </c>
+      <c r="BI9" t="s">
+        <v>44</v>
+      </c>
+      <c r="BJ9" t="s">
+        <v>40</v>
+      </c>
+      <c r="BK9" t="s">
+        <v>38</v>
+      </c>
+      <c r="BL9">
+        <v>7.5333889999999997</v>
+      </c>
+      <c r="BM9">
+        <f>_xlfn.STDEV.P(BL7:BL10)</f>
+        <v>0.18409431699997569</v>
+      </c>
+      <c r="BN9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>43</v>
       </c>
@@ -8446,8 +11431,68 @@
       <c r="G10">
         <v>8.9729109999999999</v>
       </c>
-    </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="AG10">
+        <v>11</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI10" t="s">
+        <v>33</v>
+      </c>
+      <c r="AJ10" t="s">
+        <v>39</v>
+      </c>
+      <c r="AK10">
+        <v>3.5255000000000001</v>
+      </c>
+      <c r="AP10">
+        <v>15</v>
+      </c>
+      <c r="AQ10" t="s">
+        <v>44</v>
+      </c>
+      <c r="AR10" t="s">
+        <v>40</v>
+      </c>
+      <c r="AS10" t="s">
+        <v>39</v>
+      </c>
+      <c r="AT10">
+        <v>3.1780020000000002</v>
+      </c>
+      <c r="AY10">
+        <v>11</v>
+      </c>
+      <c r="AZ10" t="s">
+        <v>44</v>
+      </c>
+      <c r="BA10" t="s">
+        <v>33</v>
+      </c>
+      <c r="BB10" t="s">
+        <v>39</v>
+      </c>
+      <c r="BC10">
+        <v>6.898752</v>
+      </c>
+      <c r="BH10">
+        <v>15</v>
+      </c>
+      <c r="BI10" t="s">
+        <v>44</v>
+      </c>
+      <c r="BJ10" t="s">
+        <v>40</v>
+      </c>
+      <c r="BK10" t="s">
+        <v>39</v>
+      </c>
+      <c r="BL10">
+        <v>7.8034150000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>43</v>
       </c>
@@ -8475,8 +11520,17 @@
       <c r="L11" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="N11" t="s">
+        <v>92</v>
+      </c>
+      <c r="O11" t="s">
+        <v>93</v>
+      </c>
+      <c r="P11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>43</v>
       </c>
@@ -8508,8 +11562,20 @@
         <f>(J2-H2)^2</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="N12">
+        <f>I2-I3</f>
+        <v>-0.21504700000000021</v>
+      </c>
+      <c r="O12" t="e">
+        <f>J2-J3</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P12" t="e">
+        <f>K2-K3</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>43</v>
       </c>
@@ -8533,8 +11599,20 @@
         <f>(J3-H3)^2</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="N13">
+        <f>I4-I5</f>
+        <v>-0.41765799999999942</v>
+      </c>
+      <c r="O13">
+        <f>J4-J5</f>
+        <v>-0.75038875000000083</v>
+      </c>
+      <c r="P13">
+        <f>K4-K5</f>
+        <v>-0.75038875000000083</v>
+      </c>
+    </row>
+    <row r="14" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>43</v>
       </c>
@@ -8562,8 +11640,20 @@
         <f t="shared" ref="L14:L19" si="2">(J4-I4)^2</f>
         <v>0.6611332362009994</v>
       </c>
-    </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="N14">
+        <f>I6-I7</f>
+        <v>-0.30866300000000102</v>
+      </c>
+      <c r="O14">
+        <f>J6-J7</f>
+        <v>-0.36883224999999875</v>
+      </c>
+      <c r="P14">
+        <f>K6-K7</f>
+        <v>-0.36883224999999875</v>
+      </c>
+    </row>
+    <row r="15" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>43</v>
       </c>
@@ -8587,8 +11677,20 @@
         <f t="shared" si="2"/>
         <v>1.3129303993080648</v>
       </c>
-    </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="N15">
+        <f>I8-I9</f>
+        <v>0.11609499999999962</v>
+      </c>
+      <c r="O15" t="e">
+        <f>J8-J9</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="P15" t="e">
+        <f>K8-K9</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="2:66" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>43</v>
       </c>
@@ -8936,8 +12038,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -9152,7 +12254,7 @@
   <dimension ref="A1:T76"/>
   <sheetViews>
     <sheetView topLeftCell="A28" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
-      <selection activeCell="P43" sqref="P43"/>
+      <selection activeCell="K59" sqref="K59:P76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
changed plot format for biox poster
</commit_message>
<xml_diff>
--- a/metaboliccostcomparisons.xlsx
+++ b/metaboliccostcomparisons.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\code\repos\Stanford\delplab\projects\muscleModel\muscleEnergyModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C148439C-E651-49F7-A899-49DB7DE3EA6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD5394A-A123-45E6-B556-1287BEE0C585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -580,6 +580,7 @@
     </indexedColors>
     <mruColors>
       <color rgb="FFFF8B8B"/>
+      <color rgb="FF2A1FFF"/>
       <color rgb="FFFF8181"/>
     </mruColors>
   </colors>
@@ -1275,20 +1276,17 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="4000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="2880" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="4000"/>
+              <a:rPr lang="en-US"/>
               <a:t>Metabolic Savings with Exotendon</a:t>
             </a:r>
           </a:p>
@@ -1307,16 +1305,13 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="4000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="2880" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -1338,9 +1333,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1">
-                <a:lumMod val="50000"/>
-              </a:schemeClr>
+              <a:srgbClr val="FF0000"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1357,22 +1350,17 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:endParaRPr lang="en-US"/>
@@ -1483,10 +1471,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1">
-                <a:lumMod val="60000"/>
-                <a:lumOff val="40000"/>
-              </a:schemeClr>
+              <a:srgbClr val="2A1FFF"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1503,22 +1488,17 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:endParaRPr lang="en-US"/>
@@ -1629,7 +1609,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="C00000"/>
+              <a:srgbClr val="FF8B8B"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1646,22 +1626,17 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:endParaRPr lang="en-US"/>
@@ -1772,7 +1747,10 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="FF8B8B"/>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1789,22 +1767,17 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:endParaRPr lang="en-US"/>
@@ -1936,20 +1909,17 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="3200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="3200"/>
+                  <a:rPr lang="en-US"/>
                   <a:t>Subjects</a:t>
                 </a:r>
               </a:p>
@@ -1976,16 +1946,13 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="3200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
               <a:endParaRPr lang="en-US"/>
@@ -2016,14 +1983,11 @@
             <a:pPr>
               <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -2066,20 +2030,17 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="4000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
+                    <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="4000"/>
+                  <a:rPr lang="en-US"/>
                   <a:t>Metabolic Power [W/kg]</a:t>
                 </a:r>
               </a:p>
@@ -2098,16 +2059,13 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="4000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
+                  <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 </a:defRPr>
               </a:pPr>
               <a:endParaRPr lang="en-US"/>
@@ -2130,16 +2088,13 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="3200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -2175,14 +2130,11 @@
           <a:pPr>
             <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -2213,7 +2165,13 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr sz="2400">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -7561,13 +7519,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>55</xdr:col>
-      <xdr:colOff>495062</xdr:colOff>
+      <xdr:colOff>495061</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>158882</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>71</xdr:col>
-      <xdr:colOff>360512</xdr:colOff>
+      <xdr:col>72</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
       <xdr:row>56</xdr:row>
       <xdr:rowOff>5801</xdr:rowOff>
     </xdr:to>
@@ -10334,7 +10292,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:BN33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AF1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AL10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="BN8" sqref="BN8:BN9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added in perc deltas for stance and swing from their respective average values
</commit_message>
<xml_diff>
--- a/metaboliccostcomparisons.xlsx
+++ b/metaboliccostcomparisons.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\code\repos\Stanford\delplab\projects\muscleModel\muscleEnergyModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5FB467DF-B679-4B07-9E04-5DC124495526}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31EAB96A-7056-46EE-8E7F-FE0B8D110CEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1110" yWindow="960" windowWidth="21600" windowHeight="11385" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="alldata" sheetId="3" r:id="rId1"/>
@@ -21,7 +21,6 @@
     <sheet name="pythonout" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="105">
   <si>
     <t>t-Test: Paired Two Sample for Means</t>
   </si>
@@ -330,9 +329,6 @@
     <t>delta percent whole</t>
   </si>
   <si>
-    <t>delta perc</t>
-  </si>
-  <si>
     <t>STDEV</t>
   </si>
   <si>
@@ -346,6 +342,15 @@
   </si>
   <si>
     <t>delta avg</t>
+  </si>
+  <si>
+    <t>delta perc whole</t>
+  </si>
+  <si>
+    <t>delta perc stance</t>
+  </si>
+  <si>
+    <t>delta perc swing</t>
   </si>
 </sst>
 </file>
@@ -7452,8 +7457,8 @@
       <xdr:rowOff>158882</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>50</xdr:col>
-      <xdr:colOff>286260</xdr:colOff>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>556723</xdr:colOff>
       <xdr:row>56</xdr:row>
       <xdr:rowOff>5801</xdr:rowOff>
     </xdr:to>
@@ -7488,8 +7493,8 @@
       <xdr:rowOff>158882</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>72</xdr:col>
-      <xdr:colOff>288102</xdr:colOff>
+      <xdr:col>71</xdr:col>
+      <xdr:colOff>205787</xdr:colOff>
       <xdr:row>56</xdr:row>
       <xdr:rowOff>5801</xdr:rowOff>
     </xdr:to>
@@ -10256,8 +10261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:BR33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" zoomScale="81" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AP13" sqref="AP13"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" zoomScale="81" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AO6" sqref="AO6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10280,6 +10285,8 @@
     <col min="17" max="17" width="29.42578125" customWidth="1"/>
     <col min="32" max="32" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="8.7109375" customWidth="1"/>
+    <col min="38" max="38" width="13.140625" customWidth="1"/>
+    <col min="39" max="39" width="13.28515625" customWidth="1"/>
     <col min="40" max="40" width="21" bestFit="1" customWidth="1"/>
     <col min="41" max="42" width="21" customWidth="1"/>
     <col min="43" max="43" width="12.85546875" bestFit="1" customWidth="1"/>
@@ -10287,8 +10294,9 @@
     <col min="57" max="57" width="30.85546875" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="59" max="59" width="7" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="61" max="62" width="13.5703125" customWidth="1"/>
+    <col min="60" max="60" width="19.85546875" customWidth="1"/>
+    <col min="61" max="61" width="17.140625" customWidth="1"/>
+    <col min="62" max="62" width="13.5703125" customWidth="1"/>
     <col min="63" max="63" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="69" max="69" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="70" max="70" width="7" bestFit="1" customWidth="1"/>
@@ -10356,10 +10364,10 @@
         <v>96</v>
       </c>
       <c r="AO1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AP1" t="s">
         <v>100</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>101</v>
       </c>
       <c r="AQ1" t="s">
         <v>88</v>
@@ -10374,13 +10382,13 @@
         <v>95</v>
       </c>
       <c r="BH1" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="BI1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="BJ1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="BK1" t="s">
         <v>90</v>
@@ -10724,6 +10732,9 @@
       <c r="AM4" t="s">
         <v>56</v>
       </c>
+      <c r="AO4" t="s">
+        <v>104</v>
+      </c>
       <c r="AR4">
         <v>5</v>
       </c>
@@ -10768,6 +10779,9 @@
       <c r="BG4" t="s">
         <v>56</v>
       </c>
+      <c r="BI4" t="s">
+        <v>103</v>
+      </c>
       <c r="BL4">
         <v>5</v>
       </c>
@@ -10859,7 +10873,11 @@
         <v>0.11590026271109134</v>
       </c>
       <c r="AM5" t="s">
-        <v>98</v>
+        <v>97</v>
+      </c>
+      <c r="AO5">
+        <f>AO3/(AVERAGE(AV3:AV10))*100</f>
+        <v>0.80763023061025396</v>
       </c>
       <c r="AR5">
         <v>6</v>
@@ -10881,7 +10899,7 @@
         <v>0.18001709462298304</v>
       </c>
       <c r="AX5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BA5">
         <v>2</v>
@@ -10903,7 +10921,11 @@
         <v>0.37912287174839515</v>
       </c>
       <c r="BG5" t="s">
-        <v>98</v>
+        <v>97</v>
+      </c>
+      <c r="BI5">
+        <f>BI3/(AVERAGE(BP3:BP10))*100</f>
+        <v>-12.506746639492015</v>
       </c>
       <c r="BL5">
         <v>6</v>
@@ -10925,7 +10947,7 @@
         <v>0.33210203248813458</v>
       </c>
       <c r="BR5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="2:70" x14ac:dyDescent="0.25">
@@ -11300,7 +11322,7 @@
         <v>0.15023717521139707</v>
       </c>
       <c r="AM9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AR9">
         <v>14</v>
@@ -11322,7 +11344,7 @@
         <v>0.11132575917858147</v>
       </c>
       <c r="AX9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BA9">
         <v>10</v>
@@ -11344,7 +11366,7 @@
         <v>0.24587854929759037</v>
       </c>
       <c r="BG9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="BL9">
         <v>14</v>
@@ -11366,7 +11388,7 @@
         <v>0.18409431699997569</v>
       </c>
       <c r="BR9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="2:70" x14ac:dyDescent="0.25">
@@ -11533,7 +11555,7 @@
         <v>-1.1394537500000013</v>
       </c>
       <c r="AM12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="2:70" x14ac:dyDescent="0.25">
@@ -11571,6 +11593,10 @@
       <c r="P13">
         <f>K4-K5</f>
         <v>-0.75038875000000083</v>
+      </c>
+      <c r="AU13">
+        <f>AVERAGE(AV3:AV10)</f>
+        <v>2.9848901249999997</v>
       </c>
     </row>
     <row r="14" spans="2:70" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
cleaning up some of the sheets
</commit_message>
<xml_diff>
--- a/metaboliccostcomparisons.xlsx
+++ b/metaboliccostcomparisons.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\code\repos\Stanford\delplab\projects\muscleModel\muscleEnergyModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{019C0958-CD14-4347-842B-5080E368A376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E5CA923-AD0B-4B49-ABCF-0E6C54FAFE50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2145" yWindow="1995" windowWidth="21600" windowHeight="11385" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="735" yWindow="735" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="alldata" sheetId="3" r:id="rId1"/>
@@ -20,8 +20,7 @@
     <sheet name="soleus_r" sheetId="13" r:id="rId5"/>
     <sheet name="pythonout" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -7830,8 +7829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:AP33"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="91" zoomScaleNormal="65" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26:F30"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10268,8 +10267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:BR33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="81" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19:P19"/>
+    <sheetView zoomScale="81" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>